<commit_message>
GFORMS-2489 - Sprint 110 release activities (#2044)
GFORMS-2489 - Sprint 110 release activities
Added the entered postcode to find the error {"obj.postcode":[{"msg":["error.invalid"],"args":[]}]}
</commit_message>
<xml_diff>
--- a/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
+++ b/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc.sharepoint.com/teams/GRP042118873/Creative Industries/Creatives Reform 2022/IT Project/Stencils/Existing reliefs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{22C6CCFF-A19B-46FE-B6E2-57F6DAA34F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1AB78D2-2A13-469D-8E8B-3891B975BABB}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{22C6CCFF-A19B-46FE-B6E2-57F6DAA34F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88969D66-D44E-46D0-9480-B1C9E9183D3F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M&amp;G Tax Relief Stencil" sheetId="2" r:id="rId1"/>
@@ -1600,33 +1600,6 @@
       <alignment horizontal="center" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1668,6 +1641,33 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2583,7 +2583,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2817,8 +2817,8 @@
   </sheetPr>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2835,25 +2835,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="119"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="110"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="122"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="113"/>
       <c r="D2" s="83" t="s">
         <v>9</v>
       </c>
@@ -2873,25 +2873,25 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="124"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="128"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="119"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="124"/>
-      <c r="C4" s="125"/>
+      <c r="B4" s="115"/>
+      <c r="C4" s="116"/>
       <c r="D4" s="25" t="s">
         <v>9</v>
       </c>
@@ -2911,11 +2911,11 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="123" t="s">
+      <c r="A5" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="124"/>
-      <c r="C5" s="125"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="116"/>
       <c r="D5" s="62"/>
       <c r="E5" s="63"/>
       <c r="F5" s="63"/>
@@ -2983,7 +2983,7 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="120" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -3001,7 +3001,7 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="108"/>
+      <c r="A10" s="120"/>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="108"/>
+      <c r="A11" s="120"/>
       <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
@@ -3033,7 +3033,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="108"/>
+      <c r="A12" s="120"/>
       <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
@@ -3061,7 +3061,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="108"/>
+      <c r="A13" s="120"/>
       <c r="B13" s="3" t="s">
         <v>37</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="20">
-        <f>SUM(F10-E12)</f>
+        <f>SUM(E11-E12)</f>
         <v>0</v>
       </c>
       <c r="F13" s="20">
@@ -3094,7 +3094,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="108"/>
+      <c r="A14" s="120"/>
       <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
@@ -3127,7 +3127,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="108"/>
+      <c r="A15" s="120"/>
       <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
@@ -3155,7 +3155,7 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="108"/>
+      <c r="A16" s="120"/>
       <c r="B16" s="3" t="s">
         <v>45</v>
       </c>
@@ -3188,7 +3188,7 @@
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="108"/>
+      <c r="A17" s="120"/>
       <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
@@ -3206,7 +3206,7 @@
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="108"/>
+      <c r="A18" s="120"/>
       <c r="B18" s="3" t="s">
         <v>51</v>
       </c>
@@ -3239,7 +3239,7 @@
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="109" t="s">
+      <c r="A19" s="121" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -3257,7 +3257,7 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="110"/>
+      <c r="A20" s="122"/>
       <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="110"/>
+      <c r="A21" s="122"/>
       <c r="B21" s="3" t="s">
         <v>59</v>
       </c>
@@ -3289,7 +3289,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="110"/>
+      <c r="A22" s="122"/>
       <c r="B22" s="3" t="s">
         <v>61</v>
       </c>
@@ -3305,7 +3305,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="110"/>
+      <c r="A23" s="122"/>
       <c r="B23" s="3" t="s">
         <v>63</v>
       </c>
@@ -3338,7 +3338,7 @@
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="110"/>
+      <c r="A24" s="122"/>
       <c r="B24" s="3" t="s">
         <v>66</v>
       </c>
@@ -3371,7 +3371,7 @@
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="110"/>
+      <c r="A25" s="122"/>
       <c r="B25" s="3" t="s">
         <v>69</v>
       </c>
@@ -3404,7 +3404,7 @@
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="110"/>
+      <c r="A26" s="122"/>
       <c r="B26" s="3" t="s">
         <v>70</v>
       </c>
@@ -3432,7 +3432,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="110"/>
+      <c r="A27" s="122"/>
       <c r="B27" s="3" t="s">
         <v>71</v>
       </c>
@@ -3465,7 +3465,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="110"/>
+      <c r="A28" s="122"/>
       <c r="B28" s="3" t="s">
         <v>72</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="111" t="s">
+      <c r="A29" s="123" t="s">
         <v>156</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -3531,7 +3531,7 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="111"/>
+      <c r="A30" s="123"/>
       <c r="B30" s="3" t="s">
         <v>158</v>
       </c>
@@ -3559,7 +3559,7 @@
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="111"/>
+      <c r="A31" s="123"/>
       <c r="B31" s="3" t="s">
         <v>160</v>
       </c>
@@ -3592,7 +3592,7 @@
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="111"/>
+      <c r="A32" s="123"/>
       <c r="B32" s="3" t="s">
         <v>163</v>
       </c>
@@ -3608,7 +3608,7 @@
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="111"/>
+      <c r="A33" s="123"/>
       <c r="B33" s="3" t="s">
         <v>164</v>
       </c>
@@ -3636,7 +3636,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="111"/>
+      <c r="A34" s="123"/>
       <c r="B34" s="3" t="s">
         <v>165</v>
       </c>
@@ -3669,7 +3669,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="111"/>
+      <c r="A35" s="123"/>
       <c r="B35" s="3" t="s">
         <v>167</v>
       </c>
@@ -3702,7 +3702,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="111"/>
+      <c r="A36" s="123"/>
       <c r="B36" s="3" t="s">
         <v>170</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="111"/>
+      <c r="A37" s="123"/>
       <c r="B37" s="3" t="s">
         <v>172</v>
       </c>
@@ -3761,7 +3761,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="111"/>
+      <c r="A38" s="123"/>
       <c r="B38" s="3" t="s">
         <v>174</v>
       </c>
@@ -3794,7 +3794,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="112" t="s">
+      <c r="A39" s="124" t="s">
         <v>81</v>
       </c>
       <c r="B39" s="89" t="s">
@@ -3814,7 +3814,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="112"/>
+      <c r="A40" s="124"/>
       <c r="B40" s="3" t="s">
         <v>85</v>
       </c>
@@ -3847,7 +3847,7 @@
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="112"/>
+      <c r="A41" s="124"/>
       <c r="B41" s="3" t="s">
         <v>87</v>
       </c>
@@ -3875,7 +3875,7 @@
       <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="112"/>
+      <c r="A42" s="124"/>
       <c r="B42" s="3" t="s">
         <v>89</v>
       </c>
@@ -3905,7 +3905,7 @@
       <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="112"/>
+      <c r="A43" s="124"/>
       <c r="B43" s="3" t="s">
         <v>91</v>
       </c>
@@ -3923,7 +3923,7 @@
       <c r="J43" s="2"/>
     </row>
     <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="112"/>
+      <c r="A44" s="124"/>
       <c r="B44" s="78" t="s">
         <v>94</v>
       </c>
@@ -3956,7 +3956,7 @@
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="112"/>
+      <c r="A45" s="124"/>
       <c r="B45" s="79" t="s">
         <v>96</v>
       </c>
@@ -3988,7 +3988,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="112"/>
+      <c r="A46" s="124"/>
       <c r="B46" s="91" t="s">
         <v>98</v>
       </c>
@@ -4020,7 +4020,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="113"/>
+      <c r="A47" s="125"/>
       <c r="B47" s="92" t="s">
         <v>100</v>
       </c>
@@ -4379,19 +4379,19 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="phAzzPOGwJOjC2+r6xrj+VDeB9u6s7Mk89S//8y0ZTl2dd/eFRKlvsNqgO56utFM91eB5TuRXJ8qH3vFKD2J4w==" saltValue="b/m4HpPV+P6zL+sDhYM3nw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="vbukBG/afY7ms7yVBfo71QQbQ9FPitRDCYfqVtnW12aeUHb7bCy7HGzaX8ZSZvWPuPkuqGp/iUP2xfyz9tuing==" saltValue="/pHJqo/0c7rBKNsnWeH4Sg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A9:A18"/>
     <mergeCell ref="A19:A28"/>
     <mergeCell ref="A29:A38"/>
     <mergeCell ref="A39:A47"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:H14">
     <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
@@ -5144,8 +5144,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="196d710fa02d7b8454006001c59ff208">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2dd5f73807ecc01be09f0551dd16e5ff" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="faf6ce0b471c2bc8070abc50707ce808">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05a7eebf91a8b30bc57d75cce2ce92d5" ns2:_="" ns3:_="">
     <xsd:import namespace="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <xsd:import namespace="7058508a-d375-4a1e-a567-7dd1bee321db"/>
     <xsd:element name="properties">
@@ -5161,6 +5176,7 @@
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5196,6 +5212,11 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="14" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="15" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -5328,36 +5349,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8774038-EE24-4DB8-A46E-183E9AA44FE8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE4759-1A60-4A08-AC49-DF59832279FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
-    <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5365,24 +5360,20 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9762069-6060-41FB-BF07-1F90D25719D4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
-    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE4759-1A60-4A08-AC49-DF59832279FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60134001-7B1A-4746-B649-C7A109D2EB68}"/>
 </file>
</xml_diff>

<commit_message>
GFORMS-2559 Resources updated to match new corrected files
</commit_message>
<xml_diff>
--- a/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
+++ b/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc.sharepoint.com/teams/GRP042118873/Creative Industries/Creatives Reform 2022/IT Project/Stencils/Existing reliefs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{22C6CCFF-A19B-46FE-B6E2-57F6DAA34F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88969D66-D44E-46D0-9480-B1C9E9183D3F}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{22C6CCFF-A19B-46FE-B6E2-57F6DAA34F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18FABB91-9BF6-46A4-92B8-40D5A227794A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11856" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M&amp;G Tax Relief Stencil" sheetId="2" r:id="rId1"/>
@@ -1600,6 +1600,42 @@
       <alignment horizontal="center" vertical="top"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1621,15 +1657,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1641,33 +1668,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1679,6 +1679,32 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2156,32 +2182,6 @@
         </patternFill>
       </fill>
       <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2274,21 +2274,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:B6" headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:B6" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27">
   <autoFilter ref="A5:B6" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Total Income" totalsRowLabel="Total" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Income of which is a State Aid" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Total Income" totalsRowLabel="Total" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Income of which is a State Aid" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A7:H46" totalsRowCount="1" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A7:H46" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22">
   <autoFilter ref="A7:H45" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2300,18 +2300,18 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Expenditure" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total expenditure" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Non Core Expenditure" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total Core Expenditure" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total UK/EEA Core Expenditure" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Total Non UK/EEA Core Expenditure" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Expenditure" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total expenditure" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Non Core Expenditure" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total Core Expenditure" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total UK/EEA Core Expenditure" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Total Non UK/EEA Core Expenditure" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUM(Table2[Total Non UK/EEA Core Expenditure])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Apportionment basis " totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Apportionment basis " totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
       <totalsRowFormula>SUM(Table2[[Apportionment basis ]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Comments" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Comments" dataDxfId="7" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2817,8 +2817,8 @@
   </sheetPr>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2835,25 +2835,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="110"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="122"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="113"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="125"/>
       <c r="D2" s="83" t="s">
         <v>9</v>
       </c>
@@ -2873,25 +2873,25 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="119"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="116"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="119"/>
       <c r="D4" s="25" t="s">
         <v>9</v>
       </c>
@@ -2911,11 +2911,11 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="114" t="s">
+      <c r="A5" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="115"/>
-      <c r="C5" s="116"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="119"/>
       <c r="D5" s="62"/>
       <c r="E5" s="63"/>
       <c r="F5" s="63"/>
@@ -2983,7 +2983,7 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="108" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -3001,7 +3001,7 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
+      <c r="A10" s="108"/>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="120"/>
+      <c r="A11" s="108"/>
       <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
@@ -3033,7 +3033,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="120"/>
+      <c r="A12" s="108"/>
       <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
@@ -3061,7 +3061,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="120"/>
+      <c r="A13" s="108"/>
       <c r="B13" s="3" t="s">
         <v>37</v>
       </c>
@@ -3094,7 +3094,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="120"/>
+      <c r="A14" s="108"/>
       <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
@@ -3106,19 +3106,19 @@
         <v>0</v>
       </c>
       <c r="E14" s="20">
-        <f>IFERROR(SUM(F10/E10*E9),0)</f>
+        <f t="shared" ref="E14:H14" si="0">IFERROR(SUM(E11/E10*E9),0)</f>
         <v>0</v>
       </c>
       <c r="F14" s="20">
-        <f>IFERROR(SUM(F11/#REF!*F9),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G14" s="20">
-        <f>IFERROR(SUM(G11/G10*G9),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="20">
-        <f>IFERROR(SUM(H11/H10*H9),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14" s="67" t="s">
@@ -3127,7 +3127,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="120"/>
+      <c r="A15" s="108"/>
       <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
@@ -3155,7 +3155,7 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="120"/>
+      <c r="A16" s="108"/>
       <c r="B16" s="3" t="s">
         <v>45</v>
       </c>
@@ -3188,7 +3188,7 @@
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="120"/>
+      <c r="A17" s="108"/>
       <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
@@ -3206,7 +3206,7 @@
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="120"/>
+      <c r="A18" s="108"/>
       <c r="B18" s="3" t="s">
         <v>51</v>
       </c>
@@ -3239,7 +3239,7 @@
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="121" t="s">
+      <c r="A19" s="109" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -3257,7 +3257,7 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="122"/>
+      <c r="A20" s="110"/>
       <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="122"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="3" t="s">
         <v>59</v>
       </c>
@@ -3289,7 +3289,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="122"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="3" t="s">
         <v>61</v>
       </c>
@@ -3305,7 +3305,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="122"/>
+      <c r="A23" s="110"/>
       <c r="B23" s="3" t="s">
         <v>63</v>
       </c>
@@ -3338,7 +3338,7 @@
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="122"/>
+      <c r="A24" s="110"/>
       <c r="B24" s="3" t="s">
         <v>66</v>
       </c>
@@ -3371,7 +3371,7 @@
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="122"/>
+      <c r="A25" s="110"/>
       <c r="B25" s="3" t="s">
         <v>69</v>
       </c>
@@ -3404,7 +3404,7 @@
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="122"/>
+      <c r="A26" s="110"/>
       <c r="B26" s="3" t="s">
         <v>70</v>
       </c>
@@ -3432,7 +3432,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="122"/>
+      <c r="A27" s="110"/>
       <c r="B27" s="3" t="s">
         <v>71</v>
       </c>
@@ -3465,7 +3465,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="122"/>
+      <c r="A28" s="110"/>
       <c r="B28" s="3" t="s">
         <v>72</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="123" t="s">
+      <c r="A29" s="111" t="s">
         <v>156</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -3531,7 +3531,7 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="123"/>
+      <c r="A30" s="111"/>
       <c r="B30" s="3" t="s">
         <v>158</v>
       </c>
@@ -3559,7 +3559,7 @@
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="123"/>
+      <c r="A31" s="111"/>
       <c r="B31" s="3" t="s">
         <v>160</v>
       </c>
@@ -3592,7 +3592,7 @@
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="123"/>
+      <c r="A32" s="111"/>
       <c r="B32" s="3" t="s">
         <v>163</v>
       </c>
@@ -3608,7 +3608,7 @@
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="123"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="3" t="s">
         <v>164</v>
       </c>
@@ -3636,7 +3636,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="123"/>
+      <c r="A34" s="111"/>
       <c r="B34" s="3" t="s">
         <v>165</v>
       </c>
@@ -3669,7 +3669,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="123"/>
+      <c r="A35" s="111"/>
       <c r="B35" s="3" t="s">
         <v>167</v>
       </c>
@@ -3702,7 +3702,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="123"/>
+      <c r="A36" s="111"/>
       <c r="B36" s="3" t="s">
         <v>170</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="123"/>
+      <c r="A37" s="111"/>
       <c r="B37" s="3" t="s">
         <v>172</v>
       </c>
@@ -3761,7 +3761,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="123"/>
+      <c r="A38" s="111"/>
       <c r="B38" s="3" t="s">
         <v>174</v>
       </c>
@@ -3794,7 +3794,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="124" t="s">
+      <c r="A39" s="112" t="s">
         <v>81</v>
       </c>
       <c r="B39" s="89" t="s">
@@ -3814,7 +3814,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="124"/>
+      <c r="A40" s="112"/>
       <c r="B40" s="3" t="s">
         <v>85</v>
       </c>
@@ -3847,7 +3847,7 @@
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="124"/>
+      <c r="A41" s="112"/>
       <c r="B41" s="3" t="s">
         <v>87</v>
       </c>
@@ -3875,14 +3875,17 @@
       <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="124"/>
+      <c r="A42" s="112"/>
       <c r="B42" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D42" s="22"/>
+      <c r="D42" s="22">
+        <f>MIN(D25-D41, ABS(D40))</f>
+        <v>0</v>
+      </c>
       <c r="E42" s="22">
         <f>MIN(E25-E41, ABS(E40))</f>
         <v>0</v>
@@ -3905,7 +3908,7 @@
       <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="124"/>
+      <c r="A43" s="112"/>
       <c r="B43" s="3" t="s">
         <v>91</v>
       </c>
@@ -3923,7 +3926,7 @@
       <c r="J43" s="2"/>
     </row>
     <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="124"/>
+      <c r="A44" s="112"/>
       <c r="B44" s="78" t="s">
         <v>94</v>
       </c>
@@ -3956,7 +3959,7 @@
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="124"/>
+      <c r="A45" s="112"/>
       <c r="B45" s="79" t="s">
         <v>96</v>
       </c>
@@ -3988,7 +3991,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="124"/>
+      <c r="A46" s="112"/>
       <c r="B46" s="91" t="s">
         <v>98</v>
       </c>
@@ -4020,7 +4023,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="125"/>
+      <c r="A47" s="113"/>
       <c r="B47" s="92" t="s">
         <v>100</v>
       </c>
@@ -4379,37 +4382,37 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vbukBG/afY7ms7yVBfo71QQbQ9FPitRDCYfqVtnW12aeUHb7bCy7HGzaX8ZSZvWPuPkuqGp/iUP2xfyz9tuing==" saltValue="/pHJqo/0c7rBKNsnWeH4Sg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jf9s6fGTqpc8Gwcnl5hiJT73225zi8qtlyT8LmDB6R79paYr5DZN0Pqm8mWrp70BSB7mKxp6Imnro/7ktG8/1g==" saltValue="Lh3Du2syQDyZsohfbRCicA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A9:A18"/>
     <mergeCell ref="A19:A28"/>
     <mergeCell ref="A29:A38"/>
     <mergeCell ref="A39:A47"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:H14">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:H14 D16:H16 D18:H18 D28:H28 D40:H40 D42:H42">
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+  <conditionalFormatting sqref="D16:H16 D18:H18 D28:H28 D40:H40 D14:H14 D42:H42">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5118,12 +5121,12 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
       <formula>$B$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5144,21 +5147,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="faf6ce0b471c2bc8070abc50707ce808">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05a7eebf91a8b30bc57d75cce2ce92d5" ns2:_="" ns3:_="">
     <xsd:import namespace="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
@@ -5349,10 +5337,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE4759-1A60-4A08-AC49-DF59832279FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60134001-7B1A-4746-B649-C7A109D2EB68}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
+    <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5360,20 +5374,24 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9762069-6060-41FB-BF07-1F90D25719D4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60134001-7B1A-4746-B649-C7A109D2EB68}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE4759-1A60-4A08-AC49-DF59832279FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GFORMS-2559 Resources updated to match new corrected files (#2048)
* GFORMS-2559 Resources updated to match new corrected files

* Worksheet snuck on
</commit_message>
<xml_diff>
--- a/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
+++ b/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc.sharepoint.com/teams/GRP042118873/Creative Industries/Creatives Reform 2022/IT Project/Stencils/Existing reliefs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{22C6CCFF-A19B-46FE-B6E2-57F6DAA34F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88969D66-D44E-46D0-9480-B1C9E9183D3F}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{22C6CCFF-A19B-46FE-B6E2-57F6DAA34F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18FABB91-9BF6-46A4-92B8-40D5A227794A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11856" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M&amp;G Tax Relief Stencil" sheetId="2" r:id="rId1"/>
@@ -1600,6 +1600,42 @@
       <alignment horizontal="center" vertical="top"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1621,15 +1657,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1641,33 +1668,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1679,6 +1679,32 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2156,32 +2182,6 @@
         </patternFill>
       </fill>
       <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2274,21 +2274,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:B6" headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:B6" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27">
   <autoFilter ref="A5:B6" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Total Income" totalsRowLabel="Total" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Income of which is a State Aid" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Total Income" totalsRowLabel="Total" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Income of which is a State Aid" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A7:H46" totalsRowCount="1" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A7:H46" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22">
   <autoFilter ref="A7:H45" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2300,18 +2300,18 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Expenditure" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total expenditure" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Non Core Expenditure" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total Core Expenditure" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total UK/EEA Core Expenditure" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Total Non UK/EEA Core Expenditure" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Expenditure" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total expenditure" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Non Core Expenditure" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total Core Expenditure" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total UK/EEA Core Expenditure" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Total Non UK/EEA Core Expenditure" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUM(Table2[Total Non UK/EEA Core Expenditure])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Apportionment basis " totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Apportionment basis " totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
       <totalsRowFormula>SUM(Table2[[Apportionment basis ]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Comments" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Comments" dataDxfId="7" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2817,8 +2817,8 @@
   </sheetPr>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2835,25 +2835,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="110"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="122"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="113"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="125"/>
       <c r="D2" s="83" t="s">
         <v>9</v>
       </c>
@@ -2873,25 +2873,25 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="119"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="116"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="119"/>
       <c r="D4" s="25" t="s">
         <v>9</v>
       </c>
@@ -2911,11 +2911,11 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="114" t="s">
+      <c r="A5" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="115"/>
-      <c r="C5" s="116"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="119"/>
       <c r="D5" s="62"/>
       <c r="E5" s="63"/>
       <c r="F5" s="63"/>
@@ -2983,7 +2983,7 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="108" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -3001,7 +3001,7 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
+      <c r="A10" s="108"/>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="120"/>
+      <c r="A11" s="108"/>
       <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
@@ -3033,7 +3033,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="120"/>
+      <c r="A12" s="108"/>
       <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
@@ -3061,7 +3061,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="120"/>
+      <c r="A13" s="108"/>
       <c r="B13" s="3" t="s">
         <v>37</v>
       </c>
@@ -3094,7 +3094,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="120"/>
+      <c r="A14" s="108"/>
       <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
@@ -3106,19 +3106,19 @@
         <v>0</v>
       </c>
       <c r="E14" s="20">
-        <f>IFERROR(SUM(F10/E10*E9),0)</f>
+        <f t="shared" ref="E14:H14" si="0">IFERROR(SUM(E11/E10*E9),0)</f>
         <v>0</v>
       </c>
       <c r="F14" s="20">
-        <f>IFERROR(SUM(F11/#REF!*F9),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G14" s="20">
-        <f>IFERROR(SUM(G11/G10*G9),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="20">
-        <f>IFERROR(SUM(H11/H10*H9),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14" s="67" t="s">
@@ -3127,7 +3127,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="120"/>
+      <c r="A15" s="108"/>
       <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
@@ -3155,7 +3155,7 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="120"/>
+      <c r="A16" s="108"/>
       <c r="B16" s="3" t="s">
         <v>45</v>
       </c>
@@ -3188,7 +3188,7 @@
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="120"/>
+      <c r="A17" s="108"/>
       <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
@@ -3206,7 +3206,7 @@
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="120"/>
+      <c r="A18" s="108"/>
       <c r="B18" s="3" t="s">
         <v>51</v>
       </c>
@@ -3239,7 +3239,7 @@
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="121" t="s">
+      <c r="A19" s="109" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -3257,7 +3257,7 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="122"/>
+      <c r="A20" s="110"/>
       <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="122"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="3" t="s">
         <v>59</v>
       </c>
@@ -3289,7 +3289,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="122"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="3" t="s">
         <v>61</v>
       </c>
@@ -3305,7 +3305,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="122"/>
+      <c r="A23" s="110"/>
       <c r="B23" s="3" t="s">
         <v>63</v>
       </c>
@@ -3338,7 +3338,7 @@
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="122"/>
+      <c r="A24" s="110"/>
       <c r="B24" s="3" t="s">
         <v>66</v>
       </c>
@@ -3371,7 +3371,7 @@
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="122"/>
+      <c r="A25" s="110"/>
       <c r="B25" s="3" t="s">
         <v>69</v>
       </c>
@@ -3404,7 +3404,7 @@
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="122"/>
+      <c r="A26" s="110"/>
       <c r="B26" s="3" t="s">
         <v>70</v>
       </c>
@@ -3432,7 +3432,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="122"/>
+      <c r="A27" s="110"/>
       <c r="B27" s="3" t="s">
         <v>71</v>
       </c>
@@ -3465,7 +3465,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="122"/>
+      <c r="A28" s="110"/>
       <c r="B28" s="3" t="s">
         <v>72</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="123" t="s">
+      <c r="A29" s="111" t="s">
         <v>156</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -3531,7 +3531,7 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="123"/>
+      <c r="A30" s="111"/>
       <c r="B30" s="3" t="s">
         <v>158</v>
       </c>
@@ -3559,7 +3559,7 @@
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="123"/>
+      <c r="A31" s="111"/>
       <c r="B31" s="3" t="s">
         <v>160</v>
       </c>
@@ -3592,7 +3592,7 @@
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="123"/>
+      <c r="A32" s="111"/>
       <c r="B32" s="3" t="s">
         <v>163</v>
       </c>
@@ -3608,7 +3608,7 @@
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="123"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="3" t="s">
         <v>164</v>
       </c>
@@ -3636,7 +3636,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="123"/>
+      <c r="A34" s="111"/>
       <c r="B34" s="3" t="s">
         <v>165</v>
       </c>
@@ -3669,7 +3669,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="123"/>
+      <c r="A35" s="111"/>
       <c r="B35" s="3" t="s">
         <v>167</v>
       </c>
@@ -3702,7 +3702,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="123"/>
+      <c r="A36" s="111"/>
       <c r="B36" s="3" t="s">
         <v>170</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="123"/>
+      <c r="A37" s="111"/>
       <c r="B37" s="3" t="s">
         <v>172</v>
       </c>
@@ -3761,7 +3761,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="123"/>
+      <c r="A38" s="111"/>
       <c r="B38" s="3" t="s">
         <v>174</v>
       </c>
@@ -3794,7 +3794,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="124" t="s">
+      <c r="A39" s="112" t="s">
         <v>81</v>
       </c>
       <c r="B39" s="89" t="s">
@@ -3814,7 +3814,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="124"/>
+      <c r="A40" s="112"/>
       <c r="B40" s="3" t="s">
         <v>85</v>
       </c>
@@ -3847,7 +3847,7 @@
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="124"/>
+      <c r="A41" s="112"/>
       <c r="B41" s="3" t="s">
         <v>87</v>
       </c>
@@ -3875,14 +3875,17 @@
       <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="124"/>
+      <c r="A42" s="112"/>
       <c r="B42" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D42" s="22"/>
+      <c r="D42" s="22">
+        <f>MIN(D25-D41, ABS(D40))</f>
+        <v>0</v>
+      </c>
       <c r="E42" s="22">
         <f>MIN(E25-E41, ABS(E40))</f>
         <v>0</v>
@@ -3905,7 +3908,7 @@
       <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="124"/>
+      <c r="A43" s="112"/>
       <c r="B43" s="3" t="s">
         <v>91</v>
       </c>
@@ -3923,7 +3926,7 @@
       <c r="J43" s="2"/>
     </row>
     <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="124"/>
+      <c r="A44" s="112"/>
       <c r="B44" s="78" t="s">
         <v>94</v>
       </c>
@@ -3956,7 +3959,7 @@
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="124"/>
+      <c r="A45" s="112"/>
       <c r="B45" s="79" t="s">
         <v>96</v>
       </c>
@@ -3988,7 +3991,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="124"/>
+      <c r="A46" s="112"/>
       <c r="B46" s="91" t="s">
         <v>98</v>
       </c>
@@ -4020,7 +4023,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="125"/>
+      <c r="A47" s="113"/>
       <c r="B47" s="92" t="s">
         <v>100</v>
       </c>
@@ -4379,37 +4382,37 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vbukBG/afY7ms7yVBfo71QQbQ9FPitRDCYfqVtnW12aeUHb7bCy7HGzaX8ZSZvWPuPkuqGp/iUP2xfyz9tuing==" saltValue="/pHJqo/0c7rBKNsnWeH4Sg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jf9s6fGTqpc8Gwcnl5hiJT73225zi8qtlyT8LmDB6R79paYr5DZN0Pqm8mWrp70BSB7mKxp6Imnro/7ktG8/1g==" saltValue="Lh3Du2syQDyZsohfbRCicA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A9:A18"/>
     <mergeCell ref="A19:A28"/>
     <mergeCell ref="A29:A38"/>
     <mergeCell ref="A39:A47"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:H14">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:H14 D16:H16 D18:H18 D28:H28 D40:H40 D42:H42">
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+  <conditionalFormatting sqref="D16:H16 D18:H18 D28:H28 D40:H40 D14:H14 D42:H42">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5118,12 +5121,12 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
       <formula>$B$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5144,21 +5147,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="faf6ce0b471c2bc8070abc50707ce808">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05a7eebf91a8b30bc57d75cce2ce92d5" ns2:_="" ns3:_="">
     <xsd:import namespace="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
@@ -5349,10 +5337,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE4759-1A60-4A08-AC49-DF59832279FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60134001-7B1A-4746-B649-C7A109D2EB68}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
+    <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5360,20 +5374,24 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9762069-6060-41FB-BF07-1F90D25719D4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60134001-7B1A-4746-B649-C7A109D2EB68}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE4759-1A60-4A08-AC49-DF59832279FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GFORMS-2559 - Resources updated to match new corrected files
</commit_message>
<xml_diff>
--- a/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
+++ b/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc.sharepoint.com/teams/GRP042118873/Creative Industries/Creatives Reform 2022/IT Project/Stencils/Existing reliefs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{22C6CCFF-A19B-46FE-B6E2-57F6DAA34F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88969D66-D44E-46D0-9480-B1C9E9183D3F}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{22C6CCFF-A19B-46FE-B6E2-57F6DAA34F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18FABB91-9BF6-46A4-92B8-40D5A227794A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11856" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M&amp;G Tax Relief Stencil" sheetId="2" r:id="rId1"/>
@@ -1600,6 +1600,42 @@
       <alignment horizontal="center" vertical="top"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1621,15 +1657,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1641,33 +1668,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1679,6 +1679,32 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2156,32 +2182,6 @@
         </patternFill>
       </fill>
       <protection locked="1" hidden="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2274,21 +2274,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:B6" headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:B6" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27">
   <autoFilter ref="A5:B6" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Total Income" totalsRowLabel="Total" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Income of which is a State Aid" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Total Income" totalsRowLabel="Total" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Income of which is a State Aid" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A7:H46" totalsRowCount="1" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A7:H46" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22">
   <autoFilter ref="A7:H45" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2300,18 +2300,18 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Expenditure" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total expenditure" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Non Core Expenditure" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total Core Expenditure" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total UK/EEA Core Expenditure" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Total Non UK/EEA Core Expenditure" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Expenditure" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total expenditure" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Non Core Expenditure" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total Core Expenditure" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total UK/EEA Core Expenditure" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Total Non UK/EEA Core Expenditure" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUM(Table2[Total Non UK/EEA Core Expenditure])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Apportionment basis " totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Apportionment basis " totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
       <totalsRowFormula>SUM(Table2[[Apportionment basis ]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Comments" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Comments" dataDxfId="7" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2817,8 +2817,8 @@
   </sheetPr>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2835,25 +2835,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="114" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="110"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="122"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="113"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="125"/>
       <c r="D2" s="83" t="s">
         <v>9</v>
       </c>
@@ -2873,25 +2873,25 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="119"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="128"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="116"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="119"/>
       <c r="D4" s="25" t="s">
         <v>9</v>
       </c>
@@ -2911,11 +2911,11 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="114" t="s">
+      <c r="A5" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="115"/>
-      <c r="C5" s="116"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="119"/>
       <c r="D5" s="62"/>
       <c r="E5" s="63"/>
       <c r="F5" s="63"/>
@@ -2983,7 +2983,7 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="108" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -3001,7 +3001,7 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
+      <c r="A10" s="108"/>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="120"/>
+      <c r="A11" s="108"/>
       <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
@@ -3033,7 +3033,7 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="120"/>
+      <c r="A12" s="108"/>
       <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
@@ -3061,7 +3061,7 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="120"/>
+      <c r="A13" s="108"/>
       <c r="B13" s="3" t="s">
         <v>37</v>
       </c>
@@ -3094,7 +3094,7 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="120"/>
+      <c r="A14" s="108"/>
       <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
@@ -3106,19 +3106,19 @@
         <v>0</v>
       </c>
       <c r="E14" s="20">
-        <f>IFERROR(SUM(F10/E10*E9),0)</f>
+        <f t="shared" ref="E14:H14" si="0">IFERROR(SUM(E11/E10*E9),0)</f>
         <v>0</v>
       </c>
       <c r="F14" s="20">
-        <f>IFERROR(SUM(F11/#REF!*F9),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G14" s="20">
-        <f>IFERROR(SUM(G11/G10*G9),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="20">
-        <f>IFERROR(SUM(H11/H10*H9),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14" s="67" t="s">
@@ -3127,7 +3127,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="120"/>
+      <c r="A15" s="108"/>
       <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
@@ -3155,7 +3155,7 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="120"/>
+      <c r="A16" s="108"/>
       <c r="B16" s="3" t="s">
         <v>45</v>
       </c>
@@ -3188,7 +3188,7 @@
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="120"/>
+      <c r="A17" s="108"/>
       <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
@@ -3206,7 +3206,7 @@
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="120"/>
+      <c r="A18" s="108"/>
       <c r="B18" s="3" t="s">
         <v>51</v>
       </c>
@@ -3239,7 +3239,7 @@
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="121" t="s">
+      <c r="A19" s="109" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -3257,7 +3257,7 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="122"/>
+      <c r="A20" s="110"/>
       <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="122"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="3" t="s">
         <v>59</v>
       </c>
@@ -3289,7 +3289,7 @@
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="122"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="3" t="s">
         <v>61</v>
       </c>
@@ -3305,7 +3305,7 @@
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="122"/>
+      <c r="A23" s="110"/>
       <c r="B23" s="3" t="s">
         <v>63</v>
       </c>
@@ -3338,7 +3338,7 @@
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="122"/>
+      <c r="A24" s="110"/>
       <c r="B24" s="3" t="s">
         <v>66</v>
       </c>
@@ -3371,7 +3371,7 @@
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="122"/>
+      <c r="A25" s="110"/>
       <c r="B25" s="3" t="s">
         <v>69</v>
       </c>
@@ -3404,7 +3404,7 @@
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="122"/>
+      <c r="A26" s="110"/>
       <c r="B26" s="3" t="s">
         <v>70</v>
       </c>
@@ -3432,7 +3432,7 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="122"/>
+      <c r="A27" s="110"/>
       <c r="B27" s="3" t="s">
         <v>71</v>
       </c>
@@ -3465,7 +3465,7 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="122"/>
+      <c r="A28" s="110"/>
       <c r="B28" s="3" t="s">
         <v>72</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="123" t="s">
+      <c r="A29" s="111" t="s">
         <v>156</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -3531,7 +3531,7 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="123"/>
+      <c r="A30" s="111"/>
       <c r="B30" s="3" t="s">
         <v>158</v>
       </c>
@@ -3559,7 +3559,7 @@
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="123"/>
+      <c r="A31" s="111"/>
       <c r="B31" s="3" t="s">
         <v>160</v>
       </c>
@@ -3592,7 +3592,7 @@
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="123"/>
+      <c r="A32" s="111"/>
       <c r="B32" s="3" t="s">
         <v>163</v>
       </c>
@@ -3608,7 +3608,7 @@
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="123"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="3" t="s">
         <v>164</v>
       </c>
@@ -3636,7 +3636,7 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="123"/>
+      <c r="A34" s="111"/>
       <c r="B34" s="3" t="s">
         <v>165</v>
       </c>
@@ -3669,7 +3669,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="123"/>
+      <c r="A35" s="111"/>
       <c r="B35" s="3" t="s">
         <v>167</v>
       </c>
@@ -3702,7 +3702,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="123"/>
+      <c r="A36" s="111"/>
       <c r="B36" s="3" t="s">
         <v>170</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="123"/>
+      <c r="A37" s="111"/>
       <c r="B37" s="3" t="s">
         <v>172</v>
       </c>
@@ -3761,7 +3761,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="123"/>
+      <c r="A38" s="111"/>
       <c r="B38" s="3" t="s">
         <v>174</v>
       </c>
@@ -3794,7 +3794,7 @@
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="124" t="s">
+      <c r="A39" s="112" t="s">
         <v>81</v>
       </c>
       <c r="B39" s="89" t="s">
@@ -3814,7 +3814,7 @@
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="124"/>
+      <c r="A40" s="112"/>
       <c r="B40" s="3" t="s">
         <v>85</v>
       </c>
@@ -3847,7 +3847,7 @@
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="124"/>
+      <c r="A41" s="112"/>
       <c r="B41" s="3" t="s">
         <v>87</v>
       </c>
@@ -3875,14 +3875,17 @@
       <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="124"/>
+      <c r="A42" s="112"/>
       <c r="B42" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D42" s="22"/>
+      <c r="D42" s="22">
+        <f>MIN(D25-D41, ABS(D40))</f>
+        <v>0</v>
+      </c>
       <c r="E42" s="22">
         <f>MIN(E25-E41, ABS(E40))</f>
         <v>0</v>
@@ -3905,7 +3908,7 @@
       <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="124"/>
+      <c r="A43" s="112"/>
       <c r="B43" s="3" t="s">
         <v>91</v>
       </c>
@@ -3923,7 +3926,7 @@
       <c r="J43" s="2"/>
     </row>
     <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="124"/>
+      <c r="A44" s="112"/>
       <c r="B44" s="78" t="s">
         <v>94</v>
       </c>
@@ -3956,7 +3959,7 @@
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="124"/>
+      <c r="A45" s="112"/>
       <c r="B45" s="79" t="s">
         <v>96</v>
       </c>
@@ -3988,7 +3991,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="124"/>
+      <c r="A46" s="112"/>
       <c r="B46" s="91" t="s">
         <v>98</v>
       </c>
@@ -4020,7 +4023,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="125"/>
+      <c r="A47" s="113"/>
       <c r="B47" s="92" t="s">
         <v>100</v>
       </c>
@@ -4379,37 +4382,37 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vbukBG/afY7ms7yVBfo71QQbQ9FPitRDCYfqVtnW12aeUHb7bCy7HGzaX8ZSZvWPuPkuqGp/iUP2xfyz9tuing==" saltValue="/pHJqo/0c7rBKNsnWeH4Sg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jf9s6fGTqpc8Gwcnl5hiJT73225zi8qtlyT8LmDB6R79paYr5DZN0Pqm8mWrp70BSB7mKxp6Imnro/7ktG8/1g==" saltValue="Lh3Du2syQDyZsohfbRCicA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A9:A18"/>
     <mergeCell ref="A19:A28"/>
     <mergeCell ref="A29:A38"/>
     <mergeCell ref="A39:A47"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:H14">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:H14 D16:H16 D18:H18 D28:H28 D40:H40 D42:H42">
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+  <conditionalFormatting sqref="D16:H16 D18:H18 D28:H28 D40:H40 D14:H14 D42:H42">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5118,12 +5121,12 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
       <formula>$B$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5144,21 +5147,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="faf6ce0b471c2bc8070abc50707ce808">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05a7eebf91a8b30bc57d75cce2ce92d5" ns2:_="" ns3:_="">
     <xsd:import namespace="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
@@ -5349,10 +5337,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE4759-1A60-4A08-AC49-DF59832279FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60134001-7B1A-4746-B649-C7A109D2EB68}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
+    <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5360,20 +5374,24 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9762069-6060-41FB-BF07-1F90D25719D4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60134001-7B1A-4746-B649-C7A109D2EB68}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE4759-1A60-4A08-AC49-DF59832279FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GFORMS-3062 Update stencils to newer versions provided on email chain
</commit_message>
<xml_diff>
--- a/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
+++ b/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc-my.sharepoint.com/personal/peter_atkins_hmrc_gov_uk/Documents/IGR/Creatives/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7209376\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{A551A379-C6F2-43DB-BDCB-8CECE4E67952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0363D7A-BE0B-4A39-8F0E-30D7EAF5D7A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58066786-7478-40EC-858B-F6D5F6B26396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M&amp;G Tax Relief Stencil" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="191">
   <si>
     <t>Museums &amp; Galleries Tax Relief Stencil</t>
   </si>
@@ -92,13 +92,13 @@
     <t>Primary or Secondary Company</t>
   </si>
   <si>
-    <t>Please Select</t>
-  </si>
-  <si>
     <t>Name of Exhibition</t>
   </si>
   <si>
     <t>Touring Or Non-touring Production</t>
+  </si>
+  <si>
+    <t>Accounting period start date</t>
   </si>
   <si>
     <t>Accounting period end (APE)</t>
@@ -414,6 +414,9 @@
     <t>TC6.1</t>
   </si>
   <si>
+    <t xml:space="preserve">M&amp;G tax credit Production start date before 27/10/2021 </t>
+  </si>
+  <si>
     <t>25% of TC5 if Touring production, otherwise 20% of TC5</t>
   </si>
   <si>
@@ -429,6 +432,12 @@
     <t>TC6.3</t>
   </si>
   <si>
+    <t>M&amp;G tax credit Productions from 01/04/2025</t>
+  </si>
+  <si>
+    <t>45% of TC5 if Touring production, otherwise 40% of TC5</t>
+  </si>
+  <si>
     <t>TC6.4</t>
   </si>
   <si>
@@ -444,12 +453,39 @@
     <t>You can find more information regarding how to calculate the relief here https://www.gov.uk/hmrc-internal-manuals/museums-and-galleries-exhibition-tax-relief/mgetr70000</t>
   </si>
   <si>
+    <t>NB 2</t>
+  </si>
+  <si>
+    <t>If your accounting period straddles 27/10/2021 or 01/04/2025, you should treat it as two notional accounting periods in this spreadsheet: the first up to that date and the second from that date.</t>
+  </si>
+  <si>
+    <t>You should apportion expenditure between the two notional periods.</t>
+  </si>
+  <si>
+    <t>NB 3</t>
+  </si>
+  <si>
+    <t>If your company has unpaid amounts brought forward, they must receive tax credit at the rate that applied in the accounting period in which they were incurred. You may have to calculate this separately.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTR &amp; MGETR  </t>
+  </si>
+  <si>
     <t>Touring</t>
   </si>
   <si>
     <t>None Touring</t>
   </si>
   <si>
+    <t>production phase date</t>
+  </si>
+  <si>
+    <t>Accoutning Period</t>
+  </si>
+  <si>
+    <t>Onward</t>
+  </si>
+  <si>
     <t>OTR</t>
   </si>
   <si>
@@ -586,45 +622,6 @@
   </si>
   <si>
     <t>NB: Expenditure not paid within 4 months of the accounting period end cannot be included in the claim.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTR &amp; MGETR  </t>
-  </si>
-  <si>
-    <t>production phase date</t>
-  </si>
-  <si>
-    <t>Accoutning Period</t>
-  </si>
-  <si>
-    <t>Onward</t>
-  </si>
-  <si>
-    <t>45% of TC5 if Touring production, otherwise 40% of TC5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M&amp;G tax credit Production start date before 27/10/2021 </t>
-  </si>
-  <si>
-    <t>M&amp;G tax credit Productions from 01/04/2025</t>
-  </si>
-  <si>
-    <t>Accounting period start date</t>
-  </si>
-  <si>
-    <t>NB 2</t>
-  </si>
-  <si>
-    <t>If your accounting period straddles 27/10/2021 or 01/04/2025, you should treat it as two notional accounting periods in this spreadsheet: the first up to that date and the second from that date.</t>
-  </si>
-  <si>
-    <t>You should apportion expenditure between the two notional periods.</t>
-  </si>
-  <si>
-    <t>NB 3</t>
-  </si>
-  <si>
-    <t>If your company has unpaid amounts brought forward, they must receive tax credit at the rate that applied in the accounting period in which they were incurred. You may have to calculate this separately.</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1289,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -1363,9 +1360,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0" hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1436,72 +1430,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1551,11 +1520,53 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
@@ -1616,27 +1627,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1649,36 +1660,45 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1688,34 +1708,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9"/>
@@ -1723,32 +1715,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2401,6 +2367,32 @@
       </fill>
       <protection locked="1" hidden="1"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2415,7 +2407,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Theatre Tax Relief Stencil"/>
@@ -2432,21 +2424,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:B6" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:B6" headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21">
   <autoFilter ref="A5:B6" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Total Income" totalsRowLabel="Total" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Income of which is a State Aid" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Total Income" totalsRowLabel="Total" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Income of which is a State Aid" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A7:H46" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A7:H46" totalsRowCount="1" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
   <autoFilter ref="A7:H45" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2458,18 +2450,18 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Expenditure" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total expenditure" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Non Core Expenditure" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total Core Expenditure" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total UK/EEA Core Expenditure" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Total Non UK/EEA Core Expenditure" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Expenditure" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total expenditure" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Non Core Expenditure" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total Core Expenditure" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total UK/EEA Core Expenditure" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Total Non UK/EEA Core Expenditure" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
       <totalsRowFormula>SUM(Table2[Total Non UK/EEA Core Expenditure])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Apportionment basis " totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Apportionment basis " totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
       <totalsRowFormula>SUM(Table2[[Apportionment basis ]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Comments" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Comments" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2761,150 +2753,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="104"/>
+      <c r="A1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="108"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
       <c r="F2" s="2"/>
       <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="105"/>
-      <c r="I2" s="106"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="110"/>
     </row>
     <row r="3" spans="1:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
       <c r="F3" s="2"/>
       <c r="G3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="105"/>
-      <c r="I3" s="106"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="110"/>
     </row>
     <row r="4" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="61"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
       <c r="J4" s="4"/>
       <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="64"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
       <c r="J5" s="4"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="101"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="64"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
       <c r="J6" s="4"/>
       <c r="K6" s="8"/>
     </row>
     <row r="7" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="64"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="64"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="63"/>
       <c r="J8" s="6"/>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="64"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="63"/>
       <c r="J9" s="6"/>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="70"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="68"/>
       <c r="J10" s="6"/>
       <c r="K10" s="7"/>
     </row>
@@ -2941,14 +2933,14 @@
   </sheetPr>
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" style="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" style="45" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="82.140625" style="11" customWidth="1"/>
     <col min="4" max="8" width="18.42578125" style="11" customWidth="1"/>
     <col min="9" max="9" width="57.5703125" style="11" customWidth="1"/>
@@ -2956,122 +2948,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="124"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="128"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="131" t="s">
+      <c r="B2" s="130"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="96"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="72"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="116" t="s">
+      <c r="B3" s="121"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="134"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="130"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="116" t="s">
+      <c r="B4" s="121"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="97"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="133" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="135"/>
-      <c r="I4" s="74"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="139" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" s="140"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-      <c r="G5" s="138"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="74"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="97"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="77"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="102"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="81"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="103"/>
     </row>
     <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="85" t="s">
+      <c r="B8" s="74"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="86" t="s">
+      <c r="E8" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="86" t="s">
+      <c r="G8" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="86" t="s">
+      <c r="H8" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="84"/>
+      <c r="I8" s="75"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
@@ -3093,7 +3081,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="18" t="s">
@@ -3110,7 +3098,7 @@
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="107"/>
+      <c r="A11" s="111"/>
       <c r="B11" s="18" t="s">
         <v>32</v>
       </c>
@@ -3125,7 +3113,7 @@
       <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="107"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="18" t="s">
         <v>34</v>
       </c>
@@ -3140,7 +3128,7 @@
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="107"/>
+      <c r="A13" s="111"/>
       <c r="B13" s="18" t="s">
         <v>36</v>
       </c>
@@ -3149,7 +3137,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="22">
-        <f>D14</f>
+        <f>D14+D13</f>
         <v>0</v>
       </c>
       <c r="F13" s="22">
@@ -3167,7 +3155,7 @@
       <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="107"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="18" t="s">
         <v>38</v>
       </c>
@@ -3199,14 +3187,14 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="107"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="20">
         <f>IFERROR(SUM(D12/D11*D10),0)</f>
         <v>0</v>
       </c>
@@ -3231,7 +3219,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="107"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="18" t="s">
         <v>44</v>
       </c>
@@ -3240,7 +3228,7 @@
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="22">
-        <f>D17</f>
+        <f>D17+D16</f>
         <v>0</v>
       </c>
       <c r="F16" s="22">
@@ -3258,30 +3246,30 @@
       <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="107"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="18" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="20">
         <f>SUM(D15-D16)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="20">
         <f>SUM(E15-E16)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="20">
         <f>SUM(F15-F16)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="20">
         <f>SUM(G15-G16)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="20">
         <f>SUM(H15-H16)</f>
         <v>0</v>
       </c>
@@ -3290,7 +3278,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="107"/>
+      <c r="A18" s="111"/>
       <c r="B18" s="18" t="s">
         <v>49</v>
       </c>
@@ -3307,30 +3295,30 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="107"/>
+      <c r="A19" s="111"/>
       <c r="B19" s="18" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="20">
         <f>SUM(D17-D14+D18)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="20">
         <f>SUM(E17-E14+E18)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="20">
         <f>SUM(F17-F14+F18)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="20">
         <f>SUM(G17-G14+G18)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="20">
         <f>SUM(H17-H14+H18)</f>
         <v>0</v>
       </c>
@@ -3339,7 +3327,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="108" t="s">
+      <c r="A20" s="112" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="18" t="s">
@@ -3356,7 +3344,7 @@
       <c r="I20" s="13"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="109"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="18" t="s">
         <v>58</v>
       </c>
@@ -3371,7 +3359,7 @@
       <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="109"/>
+      <c r="A22" s="113"/>
       <c r="B22" s="18" t="s">
         <v>60</v>
       </c>
@@ -3386,7 +3374,7 @@
       <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="109"/>
+      <c r="A23" s="113"/>
       <c r="B23" s="18" t="s">
         <v>62</v>
       </c>
@@ -3401,7 +3389,7 @@
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="109"/>
+      <c r="A24" s="113"/>
       <c r="B24" s="18" t="s">
         <v>64</v>
       </c>
@@ -3433,7 +3421,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="109"/>
+      <c r="A25" s="113"/>
       <c r="B25" s="18" t="s">
         <v>67</v>
       </c>
@@ -3465,7 +3453,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="109"/>
+      <c r="A26" s="113"/>
       <c r="B26" s="18" t="s">
         <v>70</v>
       </c>
@@ -3497,7 +3485,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="109"/>
+      <c r="A27" s="113"/>
       <c r="B27" s="18" t="s">
         <v>73</v>
       </c>
@@ -3524,7 +3512,7 @@
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="109"/>
+      <c r="A28" s="113"/>
       <c r="B28" s="18" t="s">
         <v>75</v>
       </c>
@@ -3556,30 +3544,30 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="109"/>
+      <c r="A29" s="113"/>
       <c r="B29" s="18" t="s">
         <v>78</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="23">
         <f>SUM(D19-D28)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="23">
         <f>SUM(E19-E28)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="23">
         <f>SUM(F19-F28)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="23">
         <f>SUM(G19-G28)</f>
         <v>0</v>
       </c>
-      <c r="H29" s="24">
+      <c r="H29" s="23">
         <f>SUM(H19-H28)</f>
         <v>0</v>
       </c>
@@ -3588,7 +3576,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="110" t="s">
+      <c r="A30" s="114" t="s">
         <v>81</v>
       </c>
       <c r="B30" s="18" t="s">
@@ -3620,14 +3608,14 @@
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="110"/>
+      <c r="A31" s="114"/>
       <c r="B31" s="18" t="s">
         <v>83</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="22"/>
+      <c r="D31" s="20"/>
       <c r="E31" s="22">
         <f>D30</f>
         <v>0</v>
@@ -3647,7 +3635,7 @@
       <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="110"/>
+      <c r="A32" s="114"/>
       <c r="B32" s="18" t="s">
         <v>85</v>
       </c>
@@ -3679,7 +3667,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="110"/>
+      <c r="A33" s="114"/>
       <c r="B33" s="18" t="s">
         <v>88</v>
       </c>
@@ -3691,10 +3679,10 @@
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
-      <c r="I33" s="19"/>
+      <c r="I33" s="25"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="110"/>
+      <c r="A34" s="114"/>
       <c r="B34" s="18" t="s">
         <v>90</v>
       </c>
@@ -3721,7 +3709,7 @@
       <c r="I34" s="19"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="110"/>
+      <c r="A35" s="114"/>
       <c r="B35" s="18" t="s">
         <v>92</v>
       </c>
@@ -3753,7 +3741,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="110"/>
+      <c r="A36" s="114"/>
       <c r="B36" s="18" t="s">
         <v>95</v>
       </c>
@@ -3785,7 +3773,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="110"/>
+      <c r="A37" s="114"/>
       <c r="B37" s="18" t="s">
         <v>98</v>
       </c>
@@ -3815,14 +3803,14 @@
       <c r="I37" s="19"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="110"/>
+      <c r="A38" s="114"/>
       <c r="B38" s="18" t="s">
         <v>100</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="22"/>
+      <c r="D38" s="20"/>
       <c r="E38" s="22">
         <f>D37</f>
         <v>0</v>
@@ -3842,7 +3830,7 @@
       <c r="I38" s="19"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="110"/>
+      <c r="A39" s="114"/>
       <c r="B39" s="18" t="s">
         <v>102</v>
       </c>
@@ -3874,7 +3862,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="111" t="s">
+      <c r="A40" s="115" t="s">
         <v>105</v>
       </c>
       <c r="B40" s="29" t="s">
@@ -3893,30 +3881,30 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="111"/>
+      <c r="A41" s="115"/>
       <c r="B41" s="18" t="s">
         <v>109</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41" s="23">
         <f>MIN(D29+D40, 0)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="24">
+      <c r="E41" s="23">
         <f>MIN(E29+E40, 0)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="24">
+      <c r="F41" s="23">
         <f>MIN(F29+F40, 0)</f>
         <v>0</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="23">
         <f>MIN(G29+G40, 0)</f>
         <v>0</v>
       </c>
-      <c r="H41" s="24">
+      <c r="H41" s="23">
         <f>MIN(H29+H40, 0)</f>
         <v>0</v>
       </c>
@@ -3925,7 +3913,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="111"/>
+      <c r="A42" s="115"/>
       <c r="B42" s="18" t="s">
         <v>112</v>
       </c>
@@ -3936,7 +3924,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="24">
-        <f>D44</f>
+        <f>D44+D42</f>
         <v>0</v>
       </c>
       <c r="F42" s="24">
@@ -3954,30 +3942,27 @@
       <c r="I42" s="13"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="111"/>
+      <c r="A43" s="115"/>
       <c r="B43" s="18" t="s">
         <v>114</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="24">
-        <f>MIN(D26-D42, ABS(D41))</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="24">
+      <c r="D43" s="23"/>
+      <c r="E43" s="23">
         <f>MIN(E26-E42, ABS(E41))</f>
         <v>0</v>
       </c>
-      <c r="F43" s="24">
+      <c r="F43" s="23">
         <f>MIN(F26-F42, ABS(F41))</f>
         <v>0</v>
       </c>
-      <c r="G43" s="24">
+      <c r="G43" s="23">
         <f>MIN(G26-G42, ABS(G41))</f>
         <v>0</v>
       </c>
-      <c r="H43" s="24">
+      <c r="H43" s="23">
         <f>MIN(H26-H42, ABS(H41))</f>
         <v>0</v>
       </c>
@@ -3986,15 +3971,15 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="111"/>
+      <c r="A44" s="115"/>
       <c r="B44" s="18" t="s">
         <v>117</v>
       </c>
       <c r="C44" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
       <c r="F44" s="23"/>
       <c r="G44" s="23"/>
       <c r="H44" s="23"/>
@@ -4003,12 +3988,12 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="111"/>
-      <c r="B45" s="31" t="s">
+      <c r="A45" s="115"/>
+      <c r="B45" s="30" t="s">
         <v>120</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>184</v>
+        <v>121</v>
       </c>
       <c r="D45" s="24">
         <f>SUM(D44*0.25*(D4="Touring"),D44*0.2*(D4="Non-Touring"))</f>
@@ -4031,16 +4016,16 @@
         <v>0</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="111"/>
-      <c r="B46" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C46" s="33" t="s">
+      <c r="A46" s="115"/>
+      <c r="B46" s="31" t="s">
         <v>123</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>124</v>
       </c>
       <c r="D46" s="24">
         <f>SUM(D44*0.5*(D4="Touring"),D44*0.45*(D4="Non-Touring"))</f>
@@ -4063,16 +4048,16 @@
         <v>0</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="111"/>
-      <c r="B47" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>185</v>
+      <c r="A47" s="115"/>
+      <c r="B47" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>127</v>
       </c>
       <c r="D47" s="24">
         <f>SUM(D44*0.45*(D4="Touring"),D44*0.4*(D4="Non-Touring"))</f>
@@ -4095,252 +4080,243 @@
         <v>0</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>183</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="112"/>
-      <c r="B48" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="C48" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="D48" s="37">
+      <c r="A48" s="116"/>
+      <c r="B48" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="D48" s="36">
         <f>IF(D7&lt;D66,IF(D5&gt;=D67,D47,D45),IF(D5&gt;=D67,D47,IF(D5&gt;=D66,D46,D45)))</f>
         <v>0</v>
       </c>
-      <c r="E48" s="37">
+      <c r="E48" s="36">
         <f>IF(D7&lt;D66,IF(E5&gt;=D67,E47,E45),IF(E5&gt;=D67,E47,IF(E5&gt;=D66,E46,E45)))</f>
         <v>0</v>
       </c>
-      <c r="F48" s="37">
+      <c r="F48" s="36">
         <f>IF(D7&lt;D66,IF(F5&gt;=D67,F47,F45),IF(F5&gt;=D67,F47,IF(F5&gt;=D66,F46,F45)))</f>
         <v>0</v>
       </c>
-      <c r="G48" s="37">
+      <c r="G48" s="36">
         <f>IF(D7&lt;D66,IF(G5&gt;=D67,G47,G45),IF(G5&gt;=D67,G47,IF(G5&gt;=D66,G46,G45)))</f>
         <v>0</v>
       </c>
-      <c r="H48" s="37">
+      <c r="H48" s="36">
         <f>IF(D7&lt;D66,IF(H5&gt;=D67,H47,H45),IF(H5&gt;=D67,H47,IF(H5&gt;=D66,H46,H45)))</f>
         <v>0</v>
       </c>
-      <c r="I48" s="38" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="142"/>
-      <c r="B49" s="143"/>
-      <c r="C49" s="144"/>
-      <c r="D49" s="145"/>
-      <c r="E49" s="145"/>
-      <c r="F49" s="145"/>
-      <c r="G49" s="145"/>
-      <c r="H49" s="145"/>
-      <c r="I49" s="144"/>
-    </row>
-    <row r="50" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="142"/>
-      <c r="B50" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="C50" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="D50" s="145"/>
-      <c r="E50" s="145"/>
-      <c r="F50" s="145"/>
-      <c r="G50" s="145"/>
-      <c r="H50" s="145"/>
-      <c r="I50" s="144"/>
-    </row>
-    <row r="51" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="142"/>
-      <c r="B51" s="147" t="s">
-        <v>187</v>
-      </c>
-      <c r="C51" s="148" t="s">
-        <v>188</v>
-      </c>
-      <c r="D51" s="145"/>
-      <c r="E51" s="145"/>
-      <c r="F51" s="145"/>
-      <c r="G51" s="145"/>
-      <c r="H51" s="145"/>
-      <c r="I51" s="144"/>
-    </row>
-    <row r="52" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="142"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="148" t="s">
-        <v>189</v>
-      </c>
-      <c r="D52" s="145"/>
-      <c r="E52" s="145"/>
-      <c r="F52" s="145"/>
-      <c r="G52" s="145"/>
-      <c r="H52" s="145"/>
-      <c r="I52" s="144"/>
-    </row>
-    <row r="53" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="142"/>
-      <c r="B53" s="147" t="s">
-        <v>190</v>
-      </c>
-      <c r="C53" s="148" t="s">
-        <v>191</v>
-      </c>
-      <c r="D53" s="145"/>
-      <c r="E53" s="145"/>
-      <c r="F53" s="145"/>
-      <c r="G53" s="145"/>
-      <c r="H53" s="145"/>
-      <c r="I53" s="144"/>
-    </row>
-    <row r="54" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="142"/>
-      <c r="B54" s="143"/>
-      <c r="C54" s="144"/>
-      <c r="D54" s="145"/>
-      <c r="E54" s="145"/>
-      <c r="F54" s="145"/>
-      <c r="G54" s="145"/>
-      <c r="H54" s="145"/>
-      <c r="I54" s="144"/>
-    </row>
-    <row r="55" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="142"/>
-      <c r="B55" s="143"/>
-      <c r="C55" s="144"/>
-      <c r="D55" s="145"/>
-      <c r="E55" s="145"/>
-      <c r="F55" s="145"/>
-      <c r="G55" s="145"/>
-      <c r="H55" s="145"/>
-      <c r="I55" s="144"/>
-    </row>
-    <row r="56" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="142"/>
-      <c r="B56" s="143"/>
-      <c r="C56" s="144"/>
-      <c r="D56" s="145"/>
-      <c r="E56" s="145"/>
-      <c r="F56" s="145"/>
-      <c r="G56" s="145"/>
-      <c r="H56" s="145"/>
-      <c r="I56" s="144"/>
-    </row>
-    <row r="57" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="142"/>
-      <c r="B57" s="143"/>
-      <c r="C57" s="144"/>
-      <c r="D57" s="145"/>
-      <c r="E57" s="145"/>
-      <c r="F57" s="145"/>
-      <c r="G57" s="145"/>
-      <c r="H57" s="145"/>
-      <c r="I57" s="144"/>
-    </row>
-    <row r="58" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="142"/>
-      <c r="B58" s="143"/>
-      <c r="C58" s="144"/>
-      <c r="D58" s="145"/>
-      <c r="E58" s="145"/>
-      <c r="F58" s="145"/>
-      <c r="G58" s="145"/>
-      <c r="H58" s="145"/>
-      <c r="I58" s="144"/>
-    </row>
-    <row r="59" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="142"/>
-      <c r="B59" s="143"/>
-      <c r="C59" s="144"/>
-      <c r="D59" s="145"/>
-      <c r="E59" s="145"/>
-      <c r="F59" s="145"/>
-      <c r="G59" s="145"/>
-      <c r="H59" s="145"/>
-      <c r="I59" s="144"/>
-    </row>
-    <row r="60" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="142"/>
-      <c r="B60" s="143"/>
-      <c r="C60" s="144"/>
-      <c r="D60" s="145"/>
-      <c r="E60" s="145"/>
-      <c r="F60" s="145"/>
-      <c r="G60" s="145"/>
-      <c r="H60" s="145"/>
-      <c r="I60" s="144"/>
-    </row>
-    <row r="61" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="142"/>
-      <c r="B61" s="143"/>
-      <c r="C61" s="144"/>
-      <c r="D61" s="145"/>
-      <c r="E61" s="145"/>
-      <c r="F61" s="145"/>
-      <c r="G61" s="145"/>
-      <c r="H61" s="145"/>
-      <c r="I61" s="144"/>
-    </row>
-    <row r="62" spans="1:9" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="40"/>
-      <c r="B62" s="39"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="42"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="42"/>
-      <c r="I62" s="41"/>
+      <c r="I48" s="37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="91"/>
+      <c r="C49" s="92"/>
+      <c r="D49" s="93"/>
+      <c r="E49" s="93"/>
+      <c r="F49" s="93"/>
+      <c r="G49" s="93"/>
+      <c r="H49" s="93"/>
+      <c r="I49" s="92"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="91"/>
+      <c r="B50" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="93"/>
+      <c r="E50" s="93"/>
+      <c r="F50" s="93"/>
+      <c r="G50" s="93"/>
+      <c r="H50" s="93"/>
+      <c r="I50" s="92"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="91"/>
+      <c r="B51" s="94" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="95" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="93"/>
+      <c r="E51" s="93"/>
+      <c r="F51" s="93"/>
+      <c r="G51" s="93"/>
+      <c r="H51" s="93"/>
+      <c r="I51" s="92"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="91"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="93"/>
+      <c r="E52" s="93"/>
+      <c r="F52" s="93"/>
+      <c r="G52" s="93"/>
+      <c r="H52" s="93"/>
+      <c r="I52" s="92"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="91"/>
+      <c r="B53" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="95" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="93"/>
+      <c r="E53" s="93"/>
+      <c r="F53" s="93"/>
+      <c r="G53" s="93"/>
+      <c r="H53" s="93"/>
+      <c r="I53" s="92"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="91"/>
+      <c r="C54" s="92"/>
+      <c r="D54" s="93"/>
+      <c r="E54" s="93"/>
+      <c r="F54" s="93"/>
+      <c r="G54" s="93"/>
+      <c r="H54" s="93"/>
+      <c r="I54" s="92"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="91"/>
+      <c r="C55" s="92"/>
+      <c r="D55" s="93"/>
+      <c r="E55" s="93"/>
+      <c r="F55" s="93"/>
+      <c r="G55" s="93"/>
+      <c r="H55" s="93"/>
+      <c r="I55" s="92"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="91"/>
+      <c r="C56" s="92"/>
+      <c r="D56" s="93"/>
+      <c r="E56" s="93"/>
+      <c r="F56" s="93"/>
+      <c r="G56" s="93"/>
+      <c r="H56" s="93"/>
+      <c r="I56" s="92"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="91"/>
+      <c r="C57" s="92"/>
+      <c r="D57" s="93"/>
+      <c r="E57" s="93"/>
+      <c r="F57" s="93"/>
+      <c r="G57" s="93"/>
+      <c r="H57" s="93"/>
+      <c r="I57" s="92"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="91"/>
+      <c r="C58" s="92"/>
+      <c r="D58" s="93"/>
+      <c r="E58" s="93"/>
+      <c r="F58" s="93"/>
+      <c r="G58" s="93"/>
+      <c r="H58" s="93"/>
+      <c r="I58" s="92"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="91"/>
+      <c r="C59" s="92"/>
+      <c r="D59" s="93"/>
+      <c r="E59" s="93"/>
+      <c r="F59" s="93"/>
+      <c r="G59" s="93"/>
+      <c r="H59" s="93"/>
+      <c r="I59" s="92"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="91"/>
+      <c r="C60" s="92"/>
+      <c r="D60" s="93"/>
+      <c r="E60" s="93"/>
+      <c r="F60" s="93"/>
+      <c r="G60" s="93"/>
+      <c r="H60" s="93"/>
+      <c r="I60" s="92"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="91"/>
+      <c r="C61" s="92"/>
+      <c r="D61" s="93"/>
+      <c r="E61" s="93"/>
+      <c r="F61" s="93"/>
+      <c r="G61" s="93"/>
+      <c r="H61" s="93"/>
+      <c r="I61" s="92"/>
+    </row>
+    <row r="62" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="39"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="41"/>
+      <c r="I62" s="40"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="43"/>
+      <c r="A63" s="42"/>
       <c r="B63" s="11"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="42"/>
     </row>
     <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="43"/>
-      <c r="B64" s="39"/>
-      <c r="C64" s="43"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="43"/>
+      <c r="A64" s="42"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="42"/>
+      <c r="I64" s="42"/>
     </row>
     <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="43"/>
-      <c r="B65" s="39"/>
+      <c r="A65" s="42"/>
+      <c r="B65" s="38"/>
       <c r="C65" s="5" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65"/>
       <c r="F65" s="5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H65" s="43"/>
-      <c r="I65" s="43"/>
+        <v>141</v>
+      </c>
+      <c r="H65" s="42"/>
+      <c r="I65" s="42"/>
     </row>
     <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="43"/>
-      <c r="B66" s="39"/>
+      <c r="A66" s="42"/>
+      <c r="B66" s="38"/>
       <c r="C66" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="D66" s="10">
         <v>44496</v>
@@ -4354,20 +4330,20 @@
       <c r="G66" s="5">
         <v>0.45</v>
       </c>
-      <c r="H66" s="43"/>
-      <c r="I66" s="43"/>
+      <c r="H66" s="42"/>
+      <c r="I66" s="42"/>
     </row>
     <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="43"/>
-      <c r="B67" s="39"/>
+      <c r="A67" s="42"/>
+      <c r="B67" s="38"/>
       <c r="C67" s="5" t="s">
-        <v>181</v>
+        <v>143</v>
       </c>
       <c r="D67" s="10">
         <v>45748</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="F67" s="5">
         <v>0.45</v>
@@ -4375,15 +4351,15 @@
       <c r="G67" s="5">
         <v>0.4</v>
       </c>
-      <c r="H67" s="43"/>
-      <c r="I67" s="43"/>
+      <c r="H67" s="42"/>
+      <c r="I67" s="42"/>
     </row>
     <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="D68"/>
-      <c r="E68" s="47">
+      <c r="E68" s="46">
         <v>44495</v>
       </c>
       <c r="F68">
@@ -4409,18 +4385,18 @@
     </row>
     <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71"/>
       <c r="F71" s="5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="G71" s="5"/>
     </row>
     <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="D72" s="10">
         <v>44496</v>
@@ -4439,7 +4415,7 @@
         <v>45748</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="F73" s="5">
         <v>0.45</v>
@@ -4449,7 +4425,7 @@
     <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C74"/>
       <c r="D74"/>
-      <c r="E74" s="47">
+      <c r="E74" s="46">
         <v>44495</v>
       </c>
       <c r="F74">
@@ -4459,21 +4435,21 @@
     </row>
     <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D76" s="45"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="43"/>
+      <c r="D76" s="44"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D77" s="45"/>
-      <c r="E77" s="45"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="43"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="42"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="43"/>
-      <c r="G78" s="43"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="42"/>
+      <c r="G78" s="42"/>
     </row>
     <row r="85" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D85" s="11">
@@ -4481,7 +4457,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="VFMVvvvlic6kyTxpERJC+aIFpv4jlSQBfoycG3akfkuhuMF4ucHThdbe+5J9mm6M0dt6nmQPGlvVHkpB44ZuqQ==" saltValue="EOEd2Hh/3hp7VEeveYv7hA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="CWnZTi44fG2GRBLorX1y1LeUEAUsgAuViYB2r7DA1uCR9fEi1sb6TN6EsX9nRAQB/gjDEue02bhRS4gR1dyLhg==" saltValue="RRDucwuxQSEbsBioaXto9Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="15">
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="D1:I1"/>
@@ -4500,22 +4476,22 @@
     <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D15:H15">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:H17 D19:H19 D29:H29 D41:H41 D43:H43 D15:H15">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4584,75 +4560,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="48">
+      <c r="B1" s="47">
         <f>SUM(D46,C46)</f>
         <v>0</v>
       </c>
-      <c r="E1" s="48">
+      <c r="E1" s="47">
         <f>SUM(E46,F46)</f>
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="136" t="s">
-        <v>134</v>
-      </c>
-      <c r="B2" s="136"/>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
+      <c r="A2" s="143" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="87" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="90" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="98"/>
-    </row>
-    <row r="6" spans="1:8" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="A5" s="78" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="81" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="90" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="89"/>
+    </row>
+    <row r="6" spans="1:8" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -4663,39 +4639,39 @@
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
-      <c r="H6" s="52"/>
+      <c r="H6" s="51"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" s="88" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="88" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="88" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="88" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" s="88" t="s">
-        <v>145</v>
-      </c>
-      <c r="G7" s="88" t="s">
-        <v>146</v>
-      </c>
-      <c r="H7" s="89" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="78" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="79" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="79" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="79" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" s="79" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="54"/>
+        <v>160</v>
+      </c>
+      <c r="B8" s="53"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -4703,11 +4679,11 @@
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B9" s="54"/>
+        <v>161</v>
+      </c>
+      <c r="B9" s="53"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -4715,11 +4691,11 @@
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
     </row>
-    <row r="10" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10" s="54"/>
+        <v>162</v>
+      </c>
+      <c r="B10" s="53"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -4727,11 +4703,11 @@
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
     </row>
-    <row r="11" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" s="54"/>
+        <v>163</v>
+      </c>
+      <c r="B11" s="53"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -4739,9 +4715,9 @@
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="52" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
-      <c r="B12" s="54"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -4749,9 +4725,9 @@
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
-      <c r="B13" s="54"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -4759,11 +4735,11 @@
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="B14" s="54"/>
+        <v>164</v>
+      </c>
+      <c r="B14" s="53"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
@@ -4771,11 +4747,11 @@
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B15" s="54"/>
+        <v>161</v>
+      </c>
+      <c r="B15" s="53"/>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
@@ -4783,11 +4759,11 @@
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" s="54"/>
+        <v>165</v>
+      </c>
+      <c r="B16" s="53"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
@@ -4795,11 +4771,11 @@
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" s="54"/>
+        <v>166</v>
+      </c>
+      <c r="B17" s="53"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
@@ -4807,11 +4783,11 @@
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="B18" s="54"/>
+        <v>167</v>
+      </c>
+      <c r="B18" s="53"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
@@ -4819,11 +4795,11 @@
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
     </row>
-    <row r="19" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" s="54"/>
+        <v>168</v>
+      </c>
+      <c r="B19" s="53"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
@@ -4831,11 +4807,11 @@
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
     </row>
-    <row r="20" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="B20" s="54"/>
+        <v>169</v>
+      </c>
+      <c r="B20" s="53"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
@@ -4843,11 +4819,11 @@
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
     </row>
-    <row r="21" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B21" s="54"/>
+        <v>170</v>
+      </c>
+      <c r="B21" s="53"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
@@ -4855,9 +4831,9 @@
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
     </row>
-    <row r="22" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
-      <c r="B22" s="54"/>
+      <c r="B22" s="53"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
@@ -4865,9 +4841,9 @@
       <c r="G22" s="25"/>
       <c r="H22" s="25"/>
     </row>
-    <row r="23" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
-      <c r="B23" s="54"/>
+      <c r="B23" s="53"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
@@ -4875,9 +4851,9 @@
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
     </row>
-    <row r="24" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
-      <c r="B24" s="54"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
       <c r="E24" s="25"/>
@@ -4885,9 +4861,9 @@
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
     </row>
-    <row r="25" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
-      <c r="B25" s="54"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>
       <c r="E25" s="25"/>
@@ -4895,11 +4871,11 @@
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
     </row>
-    <row r="26" spans="1:8" s="53" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
-        <v>159</v>
-      </c>
-      <c r="B26" s="54"/>
+    <row r="26" spans="1:8" s="52" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="53"/>
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>
@@ -4907,11 +4883,11 @@
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
     </row>
-    <row r="27" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" s="54"/>
+        <v>161</v>
+      </c>
+      <c r="B27" s="53"/>
       <c r="C27" s="25"/>
       <c r="D27" s="25"/>
       <c r="E27" s="25"/>
@@ -4919,11 +4895,11 @@
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="B28" s="54"/>
+        <v>172</v>
+      </c>
+      <c r="B28" s="53"/>
       <c r="C28" s="25"/>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
@@ -4931,11 +4907,11 @@
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
     </row>
-    <row r="29" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="B29" s="54"/>
+        <v>173</v>
+      </c>
+      <c r="B29" s="53"/>
       <c r="C29" s="25"/>
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>
@@ -4943,11 +4919,11 @@
       <c r="G29" s="25"/>
       <c r="H29" s="25"/>
     </row>
-    <row r="30" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="B30" s="54"/>
+        <v>174</v>
+      </c>
+      <c r="B30" s="53"/>
       <c r="C30" s="25"/>
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
@@ -4955,11 +4931,11 @@
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
     </row>
-    <row r="31" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="B31" s="54"/>
+        <v>175</v>
+      </c>
+      <c r="B31" s="53"/>
       <c r="C31" s="25"/>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
@@ -4967,11 +4943,11 @@
       <c r="G31" s="25"/>
       <c r="H31" s="25"/>
     </row>
-    <row r="32" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="B32" s="54"/>
+        <v>176</v>
+      </c>
+      <c r="B32" s="53"/>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
@@ -4979,9 +4955,9 @@
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
     </row>
-    <row r="33" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
-      <c r="B33" s="54"/>
+      <c r="B33" s="53"/>
       <c r="C33" s="25"/>
       <c r="D33" s="25"/>
       <c r="E33" s="25"/>
@@ -4989,9 +4965,9 @@
       <c r="G33" s="25"/>
       <c r="H33" s="25"/>
     </row>
-    <row r="34" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
-      <c r="B34" s="54"/>
+      <c r="B34" s="53"/>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
       <c r="E34" s="25"/>
@@ -4999,9 +4975,9 @@
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
     </row>
-    <row r="35" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
-      <c r="B35" s="54"/>
+      <c r="B35" s="53"/>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
       <c r="E35" s="25"/>
@@ -5009,11 +4985,11 @@
       <c r="G35" s="25"/>
       <c r="H35" s="25"/>
     </row>
-    <row r="36" spans="1:8" s="53" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="96" t="s">
-        <v>165</v>
-      </c>
-      <c r="B36" s="54"/>
+    <row r="36" spans="1:8" s="52" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="87" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="53"/>
       <c r="C36" s="25"/>
       <c r="D36" s="25"/>
       <c r="E36" s="25"/>
@@ -5021,11 +4997,11 @@
       <c r="G36" s="25"/>
       <c r="H36" s="25"/>
     </row>
-    <row r="37" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="B37" s="54"/>
+        <v>178</v>
+      </c>
+      <c r="B37" s="53"/>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
@@ -5033,11 +5009,11 @@
       <c r="G37" s="25"/>
       <c r="H37" s="25"/>
     </row>
-    <row r="38" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="B38" s="54"/>
+        <v>179</v>
+      </c>
+      <c r="B38" s="53"/>
       <c r="C38" s="25"/>
       <c r="D38" s="25"/>
       <c r="E38" s="25"/>
@@ -5045,11 +5021,11 @@
       <c r="G38" s="25"/>
       <c r="H38" s="25"/>
     </row>
-    <row r="39" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="B39" s="54"/>
+        <v>180</v>
+      </c>
+      <c r="B39" s="53"/>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
       <c r="E39" s="25"/>
@@ -5057,11 +5033,11 @@
       <c r="G39" s="25"/>
       <c r="H39" s="25"/>
     </row>
-    <row r="40" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="B40" s="54"/>
+        <v>181</v>
+      </c>
+      <c r="B40" s="53"/>
       <c r="C40" s="25"/>
       <c r="D40" s="25"/>
       <c r="E40" s="25"/>
@@ -5069,11 +5045,11 @@
       <c r="G40" s="25"/>
       <c r="H40" s="25"/>
     </row>
-    <row r="41" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="B41" s="54"/>
+        <v>182</v>
+      </c>
+      <c r="B41" s="53"/>
       <c r="C41" s="25"/>
       <c r="D41" s="25"/>
       <c r="E41" s="25"/>
@@ -5081,11 +5057,11 @@
       <c r="G41" s="25"/>
       <c r="H41" s="25"/>
     </row>
-    <row r="42" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="B42" s="54"/>
+        <v>183</v>
+      </c>
+      <c r="B42" s="53"/>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
       <c r="E42" s="25"/>
@@ -5093,11 +5069,11 @@
       <c r="G42" s="25"/>
       <c r="H42" s="25"/>
     </row>
-    <row r="43" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="B43" s="54"/>
+        <v>184</v>
+      </c>
+      <c r="B43" s="53"/>
       <c r="C43" s="25"/>
       <c r="D43" s="25"/>
       <c r="E43" s="25"/>
@@ -5105,11 +5081,11 @@
       <c r="G43" s="25"/>
       <c r="H43" s="25"/>
     </row>
-    <row r="44" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="B44" s="54"/>
+        <v>185</v>
+      </c>
+      <c r="B44" s="53"/>
       <c r="C44" s="25"/>
       <c r="D44" s="25"/>
       <c r="E44" s="25"/>
@@ -5117,9 +5093,9 @@
       <c r="G44" s="25"/>
       <c r="H44" s="25"/>
     </row>
-    <row r="45" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
-      <c r="B45" s="54"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="25"/>
       <c r="D45" s="25"/>
       <c r="E45" s="25"/>
@@ -5128,94 +5104,94 @@
       <c r="H45" s="25"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="91" t="s">
-        <v>174</v>
-      </c>
-      <c r="B46" s="92">
+      <c r="A46" s="82" t="s">
+        <v>186</v>
+      </c>
+      <c r="B46" s="83">
         <f>SUBTOTAL(109,Table2[Total expenditure])</f>
         <v>0</v>
       </c>
-      <c r="C46" s="92">
+      <c r="C46" s="83">
         <f>SUBTOTAL(109,Table2[Non Core Expenditure])</f>
         <v>0</v>
       </c>
-      <c r="D46" s="92">
+      <c r="D46" s="83">
         <f>SUBTOTAL(109,Table2[Total Core Expenditure])</f>
         <v>0</v>
       </c>
-      <c r="E46" s="92">
+      <c r="E46" s="83">
         <f>SUBTOTAL(109,Table2[Total UK/EEA Core Expenditure])</f>
         <v>0</v>
       </c>
-      <c r="F46" s="92">
+      <c r="F46" s="83">
         <f>SUM(Table2[Total Non UK/EEA Core Expenditure])</f>
         <v>0</v>
       </c>
-      <c r="G46" s="92">
+      <c r="G46" s="83">
         <f>SUM(Table2[[Apportionment basis ]])</f>
         <v>0</v>
       </c>
-      <c r="H46" s="93"/>
-    </row>
-    <row r="47" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="51" t="s">
-        <v>175</v>
-      </c>
-      <c r="B47" s="56"/>
+      <c r="H46" s="84"/>
+    </row>
+    <row r="47" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="50" t="s">
+        <v>187</v>
+      </c>
+      <c r="B47" s="55"/>
       <c r="C47" s="26"/>
       <c r="D47" s="26"/>
-      <c r="E47" s="57"/>
+      <c r="E47" s="56"/>
       <c r="F47" s="26"/>
       <c r="G47" s="26"/>
-      <c r="H47" s="52"/>
+      <c r="H47" s="51"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="94" t="s">
-        <v>174</v>
-      </c>
-      <c r="B48" s="95">
+      <c r="A48" s="85" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48" s="86">
         <f>Table2[[#Totals],[Total expenditure]]-B47</f>
         <v>0</v>
       </c>
-      <c r="C48" s="95">
+      <c r="C48" s="86">
         <f>Table2[[#Totals],[Non Core Expenditure]]-C47</f>
         <v>0</v>
       </c>
-      <c r="D48" s="95">
+      <c r="D48" s="86">
         <f>Table2[[#Totals],[Total Core Expenditure]]-D47</f>
         <v>0</v>
       </c>
-      <c r="E48" s="95">
+      <c r="E48" s="86">
         <f>Table2[[#Totals],[Total UK/EEA Core Expenditure]]-E47</f>
         <v>0</v>
       </c>
-      <c r="F48" s="95">
+      <c r="F48" s="86">
         <f>Table2[[#Totals],[Total Non UK/EEA Core Expenditure]]-F47</f>
         <v>0</v>
       </c>
-      <c r="G48" s="95">
+      <c r="G48" s="86">
         <f>Table2[[#Totals],[Apportionment basis ]]-G47</f>
         <v>0</v>
       </c>
-      <c r="H48" s="95"/>
+      <c r="H48" s="86"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="58"/>
+      <c r="A106" s="57"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="8zHKp46lONSTxY+OVn2QmRb5KztwPgpzj5RdsBzFdf0UAKROBjnCch+/iBXXsBaEcf5lfnOAUI9QWHt3Gtn/zw==" saltValue="lvgv5htRvjFSbAI+YtFwBg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0"/>
@@ -5224,12 +5200,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="notEqual">
       <formula>$B$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="notEqual">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5249,6 +5225,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43f61a81-08e4-450f-9189-2143ec144f36">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Notes xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
+    <Description xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
+    <Restricted_x003f_ xmlns="43f61a81-08e4-450f-9189-2143ec144f36">false</Restricted_x003f_>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Date xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
+    <_x0077_gy3 xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
+    <TaxCatchAll xmlns="229aab0b-7173-4521-96dd-bb43636f532e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5257,7 +5252,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FADE49AA34772468ECB203A2ABF3A84" ma:contentTypeVersion="31" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f4d253bc20ba4df7ac9ec746ac7562d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="43f61a81-08e4-450f-9189-2143ec144f36" xmlns:ns3="229aab0b-7173-4521-96dd-bb43636f532e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b47f16e74ed1ec9b37661be9f25fead" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5569,26 +5564,19 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43f61a81-08e4-450f-9189-2143ec144f36">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Notes xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
-    <Description xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
-    <Restricted_x003f_ xmlns="43f61a81-08e4-450f-9189-2143ec144f36">false</Restricted_x003f_>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Date xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
-    <_x0077_gy3 xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
-    <TaxCatchAll xmlns="229aab0b-7173-4521-96dd-bb43636f532e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9762069-6060-41FB-BF07-1F90D25719D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="43f61a81-08e4-450f-9189-2143ec144f36"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="229aab0b-7173-4521-96dd-bb43636f532e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE4759-1A60-4A08-AC49-DF59832279FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5596,7 +5584,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{350FA591-AFCC-4DF0-9191-454AADAFC530}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5614,22 +5602,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9762069-6060-41FB-BF07-1F90D25719D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="229aab0b-7173-4521-96dd-bb43636f532e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="43f61a81-08e4-450f-9189-2143ec144f36"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GFORMS-3062 Update stencils to newer versions provided on email chain (#2347)
</commit_message>
<xml_diff>
--- a/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
+++ b/conf/resources/museums-and-galleries-exhibition-tax-relief-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc-my.sharepoint.com/personal/peter_atkins_hmrc_gov_uk/Documents/IGR/Creatives/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7209376\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{A551A379-C6F2-43DB-BDCB-8CECE4E67952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0363D7A-BE0B-4A39-8F0E-30D7EAF5D7A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58066786-7478-40EC-858B-F6D5F6B26396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M&amp;G Tax Relief Stencil" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="191">
   <si>
     <t>Museums &amp; Galleries Tax Relief Stencil</t>
   </si>
@@ -92,13 +92,13 @@
     <t>Primary or Secondary Company</t>
   </si>
   <si>
-    <t>Please Select</t>
-  </si>
-  <si>
     <t>Name of Exhibition</t>
   </si>
   <si>
     <t>Touring Or Non-touring Production</t>
+  </si>
+  <si>
+    <t>Accounting period start date</t>
   </si>
   <si>
     <t>Accounting period end (APE)</t>
@@ -414,6 +414,9 @@
     <t>TC6.1</t>
   </si>
   <si>
+    <t xml:space="preserve">M&amp;G tax credit Production start date before 27/10/2021 </t>
+  </si>
+  <si>
     <t>25% of TC5 if Touring production, otherwise 20% of TC5</t>
   </si>
   <si>
@@ -429,6 +432,12 @@
     <t>TC6.3</t>
   </si>
   <si>
+    <t>M&amp;G tax credit Productions from 01/04/2025</t>
+  </si>
+  <si>
+    <t>45% of TC5 if Touring production, otherwise 40% of TC5</t>
+  </si>
+  <si>
     <t>TC6.4</t>
   </si>
   <si>
@@ -444,12 +453,39 @@
     <t>You can find more information regarding how to calculate the relief here https://www.gov.uk/hmrc-internal-manuals/museums-and-galleries-exhibition-tax-relief/mgetr70000</t>
   </si>
   <si>
+    <t>NB 2</t>
+  </si>
+  <si>
+    <t>If your accounting period straddles 27/10/2021 or 01/04/2025, you should treat it as two notional accounting periods in this spreadsheet: the first up to that date and the second from that date.</t>
+  </si>
+  <si>
+    <t>You should apportion expenditure between the two notional periods.</t>
+  </si>
+  <si>
+    <t>NB 3</t>
+  </si>
+  <si>
+    <t>If your company has unpaid amounts brought forward, they must receive tax credit at the rate that applied in the accounting period in which they were incurred. You may have to calculate this separately.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTR &amp; MGETR  </t>
+  </si>
+  <si>
     <t>Touring</t>
   </si>
   <si>
     <t>None Touring</t>
   </si>
   <si>
+    <t>production phase date</t>
+  </si>
+  <si>
+    <t>Accoutning Period</t>
+  </si>
+  <si>
+    <t>Onward</t>
+  </si>
+  <si>
     <t>OTR</t>
   </si>
   <si>
@@ -586,45 +622,6 @@
   </si>
   <si>
     <t>NB: Expenditure not paid within 4 months of the accounting period end cannot be included in the claim.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTR &amp; MGETR  </t>
-  </si>
-  <si>
-    <t>production phase date</t>
-  </si>
-  <si>
-    <t>Accoutning Period</t>
-  </si>
-  <si>
-    <t>Onward</t>
-  </si>
-  <si>
-    <t>45% of TC5 if Touring production, otherwise 40% of TC5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M&amp;G tax credit Production start date before 27/10/2021 </t>
-  </si>
-  <si>
-    <t>M&amp;G tax credit Productions from 01/04/2025</t>
-  </si>
-  <si>
-    <t>Accounting period start date</t>
-  </si>
-  <si>
-    <t>NB 2</t>
-  </si>
-  <si>
-    <t>If your accounting period straddles 27/10/2021 or 01/04/2025, you should treat it as two notional accounting periods in this spreadsheet: the first up to that date and the second from that date.</t>
-  </si>
-  <si>
-    <t>You should apportion expenditure between the two notional periods.</t>
-  </si>
-  <si>
-    <t>NB 3</t>
-  </si>
-  <si>
-    <t>If your company has unpaid amounts brought forward, they must receive tax credit at the rate that applied in the accounting period in which they were incurred. You may have to calculate this separately.</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1289,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -1363,9 +1360,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0" hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1436,72 +1430,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1551,11 +1520,53 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
@@ -1616,27 +1627,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1649,36 +1660,45 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1688,34 +1708,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9"/>
@@ -1723,32 +1715,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2401,6 +2367,32 @@
       </fill>
       <protection locked="1" hidden="1"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2415,7 +2407,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Theatre Tax Relief Stencil"/>
@@ -2432,21 +2424,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:B6" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:B6" headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21">
   <autoFilter ref="A5:B6" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Total Income" totalsRowLabel="Total" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Income of which is a State Aid" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Total Income" totalsRowLabel="Total" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Income of which is a State Aid" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A7:H46" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A7:H46" totalsRowCount="1" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
   <autoFilter ref="A7:H45" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2458,18 +2450,18 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Expenditure" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total expenditure" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Non Core Expenditure" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total Core Expenditure" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total UK/EEA Core Expenditure" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Total Non UK/EEA Core Expenditure" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Expenditure" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total expenditure" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Non Core Expenditure" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total Core Expenditure" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total UK/EEA Core Expenditure" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Total Non UK/EEA Core Expenditure" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
       <totalsRowFormula>SUM(Table2[Total Non UK/EEA Core Expenditure])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Apportionment basis " totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Apportionment basis " totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
       <totalsRowFormula>SUM(Table2[[Apportionment basis ]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Comments" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Comments" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2761,150 +2753,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="104"/>
+      <c r="A1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="108"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
       <c r="F2" s="2"/>
       <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="105"/>
-      <c r="I2" s="106"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="110"/>
     </row>
     <row r="3" spans="1:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
       <c r="F3" s="2"/>
       <c r="G3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="105"/>
-      <c r="I3" s="106"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="110"/>
     </row>
     <row r="4" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="61"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
       <c r="J4" s="4"/>
       <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="64"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
       <c r="J5" s="4"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="101"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="64"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
       <c r="J6" s="4"/>
       <c r="K6" s="8"/>
     </row>
     <row r="7" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="64"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="64"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="63"/>
       <c r="J8" s="6"/>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="64"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="63"/>
       <c r="J9" s="6"/>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="70"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="68"/>
       <c r="J10" s="6"/>
       <c r="K10" s="7"/>
     </row>
@@ -2941,14 +2933,14 @@
   </sheetPr>
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" style="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" style="45" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="82.140625" style="11" customWidth="1"/>
     <col min="4" max="8" width="18.42578125" style="11" customWidth="1"/>
     <col min="9" max="9" width="57.5703125" style="11" customWidth="1"/>
@@ -2956,122 +2948,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="124"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="128"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="131" t="s">
+      <c r="B2" s="130"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="96"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="72"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="116" t="s">
+      <c r="B3" s="121"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="134"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="130"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="116" t="s">
+      <c r="B4" s="121"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="97"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="133" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="135"/>
-      <c r="I4" s="74"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="139" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" s="140"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-      <c r="G5" s="138"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="74"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="97"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="77"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="102"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="81"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="103"/>
     </row>
     <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="85" t="s">
+      <c r="B8" s="74"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="86" t="s">
+      <c r="E8" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="86" t="s">
+      <c r="G8" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="86" t="s">
+      <c r="H8" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="84"/>
+      <c r="I8" s="75"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
@@ -3093,7 +3081,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="18" t="s">
@@ -3110,7 +3098,7 @@
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="107"/>
+      <c r="A11" s="111"/>
       <c r="B11" s="18" t="s">
         <v>32</v>
       </c>
@@ -3125,7 +3113,7 @@
       <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="107"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="18" t="s">
         <v>34</v>
       </c>
@@ -3140,7 +3128,7 @@
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="107"/>
+      <c r="A13" s="111"/>
       <c r="B13" s="18" t="s">
         <v>36</v>
       </c>
@@ -3149,7 +3137,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="22">
-        <f>D14</f>
+        <f>D14+D13</f>
         <v>0</v>
       </c>
       <c r="F13" s="22">
@@ -3167,7 +3155,7 @@
       <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="107"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="18" t="s">
         <v>38</v>
       </c>
@@ -3199,14 +3187,14 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="107"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="20">
         <f>IFERROR(SUM(D12/D11*D10),0)</f>
         <v>0</v>
       </c>
@@ -3231,7 +3219,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="107"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="18" t="s">
         <v>44</v>
       </c>
@@ -3240,7 +3228,7 @@
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="22">
-        <f>D17</f>
+        <f>D17+D16</f>
         <v>0</v>
       </c>
       <c r="F16" s="22">
@@ -3258,30 +3246,30 @@
       <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="107"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="18" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="20">
         <f>SUM(D15-D16)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="20">
         <f>SUM(E15-E16)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="20">
         <f>SUM(F15-F16)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="20">
         <f>SUM(G15-G16)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="20">
         <f>SUM(H15-H16)</f>
         <v>0</v>
       </c>
@@ -3290,7 +3278,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="107"/>
+      <c r="A18" s="111"/>
       <c r="B18" s="18" t="s">
         <v>49</v>
       </c>
@@ -3307,30 +3295,30 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="107"/>
+      <c r="A19" s="111"/>
       <c r="B19" s="18" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="20">
         <f>SUM(D17-D14+D18)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="20">
         <f>SUM(E17-E14+E18)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="20">
         <f>SUM(F17-F14+F18)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="20">
         <f>SUM(G17-G14+G18)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="20">
         <f>SUM(H17-H14+H18)</f>
         <v>0</v>
       </c>
@@ -3339,7 +3327,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="108" t="s">
+      <c r="A20" s="112" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="18" t="s">
@@ -3356,7 +3344,7 @@
       <c r="I20" s="13"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="109"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="18" t="s">
         <v>58</v>
       </c>
@@ -3371,7 +3359,7 @@
       <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="109"/>
+      <c r="A22" s="113"/>
       <c r="B22" s="18" t="s">
         <v>60</v>
       </c>
@@ -3386,7 +3374,7 @@
       <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="109"/>
+      <c r="A23" s="113"/>
       <c r="B23" s="18" t="s">
         <v>62</v>
       </c>
@@ -3401,7 +3389,7 @@
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="109"/>
+      <c r="A24" s="113"/>
       <c r="B24" s="18" t="s">
         <v>64</v>
       </c>
@@ -3433,7 +3421,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="109"/>
+      <c r="A25" s="113"/>
       <c r="B25" s="18" t="s">
         <v>67</v>
       </c>
@@ -3465,7 +3453,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="109"/>
+      <c r="A26" s="113"/>
       <c r="B26" s="18" t="s">
         <v>70</v>
       </c>
@@ -3497,7 +3485,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="109"/>
+      <c r="A27" s="113"/>
       <c r="B27" s="18" t="s">
         <v>73</v>
       </c>
@@ -3524,7 +3512,7 @@
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="109"/>
+      <c r="A28" s="113"/>
       <c r="B28" s="18" t="s">
         <v>75</v>
       </c>
@@ -3556,30 +3544,30 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="109"/>
+      <c r="A29" s="113"/>
       <c r="B29" s="18" t="s">
         <v>78</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="23">
         <f>SUM(D19-D28)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="23">
         <f>SUM(E19-E28)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="23">
         <f>SUM(F19-F28)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="23">
         <f>SUM(G19-G28)</f>
         <v>0</v>
       </c>
-      <c r="H29" s="24">
+      <c r="H29" s="23">
         <f>SUM(H19-H28)</f>
         <v>0</v>
       </c>
@@ -3588,7 +3576,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="110" t="s">
+      <c r="A30" s="114" t="s">
         <v>81</v>
       </c>
       <c r="B30" s="18" t="s">
@@ -3620,14 +3608,14 @@
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="110"/>
+      <c r="A31" s="114"/>
       <c r="B31" s="18" t="s">
         <v>83</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="22"/>
+      <c r="D31" s="20"/>
       <c r="E31" s="22">
         <f>D30</f>
         <v>0</v>
@@ -3647,7 +3635,7 @@
       <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="110"/>
+      <c r="A32" s="114"/>
       <c r="B32" s="18" t="s">
         <v>85</v>
       </c>
@@ -3679,7 +3667,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="110"/>
+      <c r="A33" s="114"/>
       <c r="B33" s="18" t="s">
         <v>88</v>
       </c>
@@ -3691,10 +3679,10 @@
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
-      <c r="I33" s="19"/>
+      <c r="I33" s="25"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="110"/>
+      <c r="A34" s="114"/>
       <c r="B34" s="18" t="s">
         <v>90</v>
       </c>
@@ -3721,7 +3709,7 @@
       <c r="I34" s="19"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="110"/>
+      <c r="A35" s="114"/>
       <c r="B35" s="18" t="s">
         <v>92</v>
       </c>
@@ -3753,7 +3741,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="110"/>
+      <c r="A36" s="114"/>
       <c r="B36" s="18" t="s">
         <v>95</v>
       </c>
@@ -3785,7 +3773,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="110"/>
+      <c r="A37" s="114"/>
       <c r="B37" s="18" t="s">
         <v>98</v>
       </c>
@@ -3815,14 +3803,14 @@
       <c r="I37" s="19"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="110"/>
+      <c r="A38" s="114"/>
       <c r="B38" s="18" t="s">
         <v>100</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="22"/>
+      <c r="D38" s="20"/>
       <c r="E38" s="22">
         <f>D37</f>
         <v>0</v>
@@ -3842,7 +3830,7 @@
       <c r="I38" s="19"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="110"/>
+      <c r="A39" s="114"/>
       <c r="B39" s="18" t="s">
         <v>102</v>
       </c>
@@ -3874,7 +3862,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="111" t="s">
+      <c r="A40" s="115" t="s">
         <v>105</v>
       </c>
       <c r="B40" s="29" t="s">
@@ -3893,30 +3881,30 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="111"/>
+      <c r="A41" s="115"/>
       <c r="B41" s="18" t="s">
         <v>109</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41" s="23">
         <f>MIN(D29+D40, 0)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="24">
+      <c r="E41" s="23">
         <f>MIN(E29+E40, 0)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="24">
+      <c r="F41" s="23">
         <f>MIN(F29+F40, 0)</f>
         <v>0</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="23">
         <f>MIN(G29+G40, 0)</f>
         <v>0</v>
       </c>
-      <c r="H41" s="24">
+      <c r="H41" s="23">
         <f>MIN(H29+H40, 0)</f>
         <v>0</v>
       </c>
@@ -3925,7 +3913,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="111"/>
+      <c r="A42" s="115"/>
       <c r="B42" s="18" t="s">
         <v>112</v>
       </c>
@@ -3936,7 +3924,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="24">
-        <f>D44</f>
+        <f>D44+D42</f>
         <v>0</v>
       </c>
       <c r="F42" s="24">
@@ -3954,30 +3942,27 @@
       <c r="I42" s="13"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="111"/>
+      <c r="A43" s="115"/>
       <c r="B43" s="18" t="s">
         <v>114</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="24">
-        <f>MIN(D26-D42, ABS(D41))</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="24">
+      <c r="D43" s="23"/>
+      <c r="E43" s="23">
         <f>MIN(E26-E42, ABS(E41))</f>
         <v>0</v>
       </c>
-      <c r="F43" s="24">
+      <c r="F43" s="23">
         <f>MIN(F26-F42, ABS(F41))</f>
         <v>0</v>
       </c>
-      <c r="G43" s="24">
+      <c r="G43" s="23">
         <f>MIN(G26-G42, ABS(G41))</f>
         <v>0</v>
       </c>
-      <c r="H43" s="24">
+      <c r="H43" s="23">
         <f>MIN(H26-H42, ABS(H41))</f>
         <v>0</v>
       </c>
@@ -3986,15 +3971,15 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="111"/>
+      <c r="A44" s="115"/>
       <c r="B44" s="18" t="s">
         <v>117</v>
       </c>
       <c r="C44" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
       <c r="F44" s="23"/>
       <c r="G44" s="23"/>
       <c r="H44" s="23"/>
@@ -4003,12 +3988,12 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="111"/>
-      <c r="B45" s="31" t="s">
+      <c r="A45" s="115"/>
+      <c r="B45" s="30" t="s">
         <v>120</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>184</v>
+        <v>121</v>
       </c>
       <c r="D45" s="24">
         <f>SUM(D44*0.25*(D4="Touring"),D44*0.2*(D4="Non-Touring"))</f>
@@ -4031,16 +4016,16 @@
         <v>0</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="111"/>
-      <c r="B46" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="C46" s="33" t="s">
+      <c r="A46" s="115"/>
+      <c r="B46" s="31" t="s">
         <v>123</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>124</v>
       </c>
       <c r="D46" s="24">
         <f>SUM(D44*0.5*(D4="Touring"),D44*0.45*(D4="Non-Touring"))</f>
@@ -4063,16 +4048,16 @@
         <v>0</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="111"/>
-      <c r="B47" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>185</v>
+      <c r="A47" s="115"/>
+      <c r="B47" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>127</v>
       </c>
       <c r="D47" s="24">
         <f>SUM(D44*0.45*(D4="Touring"),D44*0.4*(D4="Non-Touring"))</f>
@@ -4095,252 +4080,243 @@
         <v>0</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>183</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="112"/>
-      <c r="B48" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="C48" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="D48" s="37">
+      <c r="A48" s="116"/>
+      <c r="B48" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="D48" s="36">
         <f>IF(D7&lt;D66,IF(D5&gt;=D67,D47,D45),IF(D5&gt;=D67,D47,IF(D5&gt;=D66,D46,D45)))</f>
         <v>0</v>
       </c>
-      <c r="E48" s="37">
+      <c r="E48" s="36">
         <f>IF(D7&lt;D66,IF(E5&gt;=D67,E47,E45),IF(E5&gt;=D67,E47,IF(E5&gt;=D66,E46,E45)))</f>
         <v>0</v>
       </c>
-      <c r="F48" s="37">
+      <c r="F48" s="36">
         <f>IF(D7&lt;D66,IF(F5&gt;=D67,F47,F45),IF(F5&gt;=D67,F47,IF(F5&gt;=D66,F46,F45)))</f>
         <v>0</v>
       </c>
-      <c r="G48" s="37">
+      <c r="G48" s="36">
         <f>IF(D7&lt;D66,IF(G5&gt;=D67,G47,G45),IF(G5&gt;=D67,G47,IF(G5&gt;=D66,G46,G45)))</f>
         <v>0</v>
       </c>
-      <c r="H48" s="37">
+      <c r="H48" s="36">
         <f>IF(D7&lt;D66,IF(H5&gt;=D67,H47,H45),IF(H5&gt;=D67,H47,IF(H5&gt;=D66,H46,H45)))</f>
         <v>0</v>
       </c>
-      <c r="I48" s="38" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="142"/>
-      <c r="B49" s="143"/>
-      <c r="C49" s="144"/>
-      <c r="D49" s="145"/>
-      <c r="E49" s="145"/>
-      <c r="F49" s="145"/>
-      <c r="G49" s="145"/>
-      <c r="H49" s="145"/>
-      <c r="I49" s="144"/>
-    </row>
-    <row r="50" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="142"/>
-      <c r="B50" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="C50" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="D50" s="145"/>
-      <c r="E50" s="145"/>
-      <c r="F50" s="145"/>
-      <c r="G50" s="145"/>
-      <c r="H50" s="145"/>
-      <c r="I50" s="144"/>
-    </row>
-    <row r="51" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="142"/>
-      <c r="B51" s="147" t="s">
-        <v>187</v>
-      </c>
-      <c r="C51" s="148" t="s">
-        <v>188</v>
-      </c>
-      <c r="D51" s="145"/>
-      <c r="E51" s="145"/>
-      <c r="F51" s="145"/>
-      <c r="G51" s="145"/>
-      <c r="H51" s="145"/>
-      <c r="I51" s="144"/>
-    </row>
-    <row r="52" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="142"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="148" t="s">
-        <v>189</v>
-      </c>
-      <c r="D52" s="145"/>
-      <c r="E52" s="145"/>
-      <c r="F52" s="145"/>
-      <c r="G52" s="145"/>
-      <c r="H52" s="145"/>
-      <c r="I52" s="144"/>
-    </row>
-    <row r="53" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="142"/>
-      <c r="B53" s="147" t="s">
-        <v>190</v>
-      </c>
-      <c r="C53" s="148" t="s">
-        <v>191</v>
-      </c>
-      <c r="D53" s="145"/>
-      <c r="E53" s="145"/>
-      <c r="F53" s="145"/>
-      <c r="G53" s="145"/>
-      <c r="H53" s="145"/>
-      <c r="I53" s="144"/>
-    </row>
-    <row r="54" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="142"/>
-      <c r="B54" s="143"/>
-      <c r="C54" s="144"/>
-      <c r="D54" s="145"/>
-      <c r="E54" s="145"/>
-      <c r="F54" s="145"/>
-      <c r="G54" s="145"/>
-      <c r="H54" s="145"/>
-      <c r="I54" s="144"/>
-    </row>
-    <row r="55" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="142"/>
-      <c r="B55" s="143"/>
-      <c r="C55" s="144"/>
-      <c r="D55" s="145"/>
-      <c r="E55" s="145"/>
-      <c r="F55" s="145"/>
-      <c r="G55" s="145"/>
-      <c r="H55" s="145"/>
-      <c r="I55" s="144"/>
-    </row>
-    <row r="56" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="142"/>
-      <c r="B56" s="143"/>
-      <c r="C56" s="144"/>
-      <c r="D56" s="145"/>
-      <c r="E56" s="145"/>
-      <c r="F56" s="145"/>
-      <c r="G56" s="145"/>
-      <c r="H56" s="145"/>
-      <c r="I56" s="144"/>
-    </row>
-    <row r="57" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="142"/>
-      <c r="B57" s="143"/>
-      <c r="C57" s="144"/>
-      <c r="D57" s="145"/>
-      <c r="E57" s="145"/>
-      <c r="F57" s="145"/>
-      <c r="G57" s="145"/>
-      <c r="H57" s="145"/>
-      <c r="I57" s="144"/>
-    </row>
-    <row r="58" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="142"/>
-      <c r="B58" s="143"/>
-      <c r="C58" s="144"/>
-      <c r="D58" s="145"/>
-      <c r="E58" s="145"/>
-      <c r="F58" s="145"/>
-      <c r="G58" s="145"/>
-      <c r="H58" s="145"/>
-      <c r="I58" s="144"/>
-    </row>
-    <row r="59" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="142"/>
-      <c r="B59" s="143"/>
-      <c r="C59" s="144"/>
-      <c r="D59" s="145"/>
-      <c r="E59" s="145"/>
-      <c r="F59" s="145"/>
-      <c r="G59" s="145"/>
-      <c r="H59" s="145"/>
-      <c r="I59" s="144"/>
-    </row>
-    <row r="60" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="142"/>
-      <c r="B60" s="143"/>
-      <c r="C60" s="144"/>
-      <c r="D60" s="145"/>
-      <c r="E60" s="145"/>
-      <c r="F60" s="145"/>
-      <c r="G60" s="145"/>
-      <c r="H60" s="145"/>
-      <c r="I60" s="144"/>
-    </row>
-    <row r="61" spans="1:9" s="146" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="142"/>
-      <c r="B61" s="143"/>
-      <c r="C61" s="144"/>
-      <c r="D61" s="145"/>
-      <c r="E61" s="145"/>
-      <c r="F61" s="145"/>
-      <c r="G61" s="145"/>
-      <c r="H61" s="145"/>
-      <c r="I61" s="144"/>
-    </row>
-    <row r="62" spans="1:9" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="40"/>
-      <c r="B62" s="39"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="42"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="42"/>
-      <c r="I62" s="41"/>
+      <c r="I48" s="37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="91"/>
+      <c r="C49" s="92"/>
+      <c r="D49" s="93"/>
+      <c r="E49" s="93"/>
+      <c r="F49" s="93"/>
+      <c r="G49" s="93"/>
+      <c r="H49" s="93"/>
+      <c r="I49" s="92"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="91"/>
+      <c r="B50" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="93"/>
+      <c r="E50" s="93"/>
+      <c r="F50" s="93"/>
+      <c r="G50" s="93"/>
+      <c r="H50" s="93"/>
+      <c r="I50" s="92"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="91"/>
+      <c r="B51" s="94" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="95" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="93"/>
+      <c r="E51" s="93"/>
+      <c r="F51" s="93"/>
+      <c r="G51" s="93"/>
+      <c r="H51" s="93"/>
+      <c r="I51" s="92"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="91"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="93"/>
+      <c r="E52" s="93"/>
+      <c r="F52" s="93"/>
+      <c r="G52" s="93"/>
+      <c r="H52" s="93"/>
+      <c r="I52" s="92"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="91"/>
+      <c r="B53" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="95" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="93"/>
+      <c r="E53" s="93"/>
+      <c r="F53" s="93"/>
+      <c r="G53" s="93"/>
+      <c r="H53" s="93"/>
+      <c r="I53" s="92"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="91"/>
+      <c r="C54" s="92"/>
+      <c r="D54" s="93"/>
+      <c r="E54" s="93"/>
+      <c r="F54" s="93"/>
+      <c r="G54" s="93"/>
+      <c r="H54" s="93"/>
+      <c r="I54" s="92"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="91"/>
+      <c r="C55" s="92"/>
+      <c r="D55" s="93"/>
+      <c r="E55" s="93"/>
+      <c r="F55" s="93"/>
+      <c r="G55" s="93"/>
+      <c r="H55" s="93"/>
+      <c r="I55" s="92"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="91"/>
+      <c r="C56" s="92"/>
+      <c r="D56" s="93"/>
+      <c r="E56" s="93"/>
+      <c r="F56" s="93"/>
+      <c r="G56" s="93"/>
+      <c r="H56" s="93"/>
+      <c r="I56" s="92"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="91"/>
+      <c r="C57" s="92"/>
+      <c r="D57" s="93"/>
+      <c r="E57" s="93"/>
+      <c r="F57" s="93"/>
+      <c r="G57" s="93"/>
+      <c r="H57" s="93"/>
+      <c r="I57" s="92"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="91"/>
+      <c r="C58" s="92"/>
+      <c r="D58" s="93"/>
+      <c r="E58" s="93"/>
+      <c r="F58" s="93"/>
+      <c r="G58" s="93"/>
+      <c r="H58" s="93"/>
+      <c r="I58" s="92"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="91"/>
+      <c r="C59" s="92"/>
+      <c r="D59" s="93"/>
+      <c r="E59" s="93"/>
+      <c r="F59" s="93"/>
+      <c r="G59" s="93"/>
+      <c r="H59" s="93"/>
+      <c r="I59" s="92"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="91"/>
+      <c r="C60" s="92"/>
+      <c r="D60" s="93"/>
+      <c r="E60" s="93"/>
+      <c r="F60" s="93"/>
+      <c r="G60" s="93"/>
+      <c r="H60" s="93"/>
+      <c r="I60" s="92"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="91"/>
+      <c r="C61" s="92"/>
+      <c r="D61" s="93"/>
+      <c r="E61" s="93"/>
+      <c r="F61" s="93"/>
+      <c r="G61" s="93"/>
+      <c r="H61" s="93"/>
+      <c r="I61" s="92"/>
+    </row>
+    <row r="62" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="39"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="41"/>
+      <c r="I62" s="40"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="43"/>
+      <c r="A63" s="42"/>
       <c r="B63" s="11"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="42"/>
     </row>
     <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="43"/>
-      <c r="B64" s="39"/>
-      <c r="C64" s="43"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="43"/>
+      <c r="A64" s="42"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="42"/>
+      <c r="I64" s="42"/>
     </row>
     <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="43"/>
-      <c r="B65" s="39"/>
+      <c r="A65" s="42"/>
+      <c r="B65" s="38"/>
       <c r="C65" s="5" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65"/>
       <c r="F65" s="5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H65" s="43"/>
-      <c r="I65" s="43"/>
+        <v>141</v>
+      </c>
+      <c r="H65" s="42"/>
+      <c r="I65" s="42"/>
     </row>
     <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="43"/>
-      <c r="B66" s="39"/>
+      <c r="A66" s="42"/>
+      <c r="B66" s="38"/>
       <c r="C66" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="D66" s="10">
         <v>44496</v>
@@ -4354,20 +4330,20 @@
       <c r="G66" s="5">
         <v>0.45</v>
       </c>
-      <c r="H66" s="43"/>
-      <c r="I66" s="43"/>
+      <c r="H66" s="42"/>
+      <c r="I66" s="42"/>
     </row>
     <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="43"/>
-      <c r="B67" s="39"/>
+      <c r="A67" s="42"/>
+      <c r="B67" s="38"/>
       <c r="C67" s="5" t="s">
-        <v>181</v>
+        <v>143</v>
       </c>
       <c r="D67" s="10">
         <v>45748</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="F67" s="5">
         <v>0.45</v>
@@ -4375,15 +4351,15 @@
       <c r="G67" s="5">
         <v>0.4</v>
       </c>
-      <c r="H67" s="43"/>
-      <c r="I67" s="43"/>
+      <c r="H67" s="42"/>
+      <c r="I67" s="42"/>
     </row>
     <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="D68"/>
-      <c r="E68" s="47">
+      <c r="E68" s="46">
         <v>44495</v>
       </c>
       <c r="F68">
@@ -4409,18 +4385,18 @@
     </row>
     <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71"/>
       <c r="F71" s="5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="G71" s="5"/>
     </row>
     <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="D72" s="10">
         <v>44496</v>
@@ -4439,7 +4415,7 @@
         <v>45748</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="F73" s="5">
         <v>0.45</v>
@@ -4449,7 +4425,7 @@
     <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C74"/>
       <c r="D74"/>
-      <c r="E74" s="47">
+      <c r="E74" s="46">
         <v>44495</v>
       </c>
       <c r="F74">
@@ -4459,21 +4435,21 @@
     </row>
     <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D76" s="45"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="43"/>
+      <c r="D76" s="44"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D77" s="45"/>
-      <c r="E77" s="45"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="43"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="42"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="43"/>
-      <c r="G78" s="43"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="42"/>
+      <c r="G78" s="42"/>
     </row>
     <row r="85" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="D85" s="11">
@@ -4481,7 +4457,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="VFMVvvvlic6kyTxpERJC+aIFpv4jlSQBfoycG3akfkuhuMF4ucHThdbe+5J9mm6M0dt6nmQPGlvVHkpB44ZuqQ==" saltValue="EOEd2Hh/3hp7VEeveYv7hA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="CWnZTi44fG2GRBLorX1y1LeUEAUsgAuViYB2r7DA1uCR9fEi1sb6TN6EsX9nRAQB/gjDEue02bhRS4gR1dyLhg==" saltValue="RRDucwuxQSEbsBioaXto9Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="15">
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="D1:I1"/>
@@ -4500,22 +4476,22 @@
     <mergeCell ref="A6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D15:H15">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:H17 D19:H19 D29:H29 D41:H41 D43:H43 D15:H15">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4584,75 +4560,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="48">
+      <c r="B1" s="47">
         <f>SUM(D46,C46)</f>
         <v>0</v>
       </c>
-      <c r="E1" s="48">
+      <c r="E1" s="47">
         <f>SUM(E46,F46)</f>
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="136" t="s">
-        <v>134</v>
-      </c>
-      <c r="B2" s="136"/>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
+      <c r="A2" s="143" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="87" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="90" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="99" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="98"/>
-    </row>
-    <row r="6" spans="1:8" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="A5" s="78" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="81" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="90" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="89"/>
+    </row>
+    <row r="6" spans="1:8" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -4663,39 +4639,39 @@
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
-      <c r="H6" s="52"/>
+      <c r="H6" s="51"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" s="88" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="88" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="88" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="88" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" s="88" t="s">
-        <v>145</v>
-      </c>
-      <c r="G7" s="88" t="s">
-        <v>146</v>
-      </c>
-      <c r="H7" s="89" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="78" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="79" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="79" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="79" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" s="79" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="54"/>
+        <v>160</v>
+      </c>
+      <c r="B8" s="53"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -4703,11 +4679,11 @@
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B9" s="54"/>
+        <v>161</v>
+      </c>
+      <c r="B9" s="53"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -4715,11 +4691,11 @@
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
     </row>
-    <row r="10" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10" s="54"/>
+        <v>162</v>
+      </c>
+      <c r="B10" s="53"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -4727,11 +4703,11 @@
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
     </row>
-    <row r="11" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" s="54"/>
+        <v>163</v>
+      </c>
+      <c r="B11" s="53"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -4739,9 +4715,9 @@
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="52" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
-      <c r="B12" s="54"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -4749,9 +4725,9 @@
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
-      <c r="B13" s="54"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -4759,11 +4735,11 @@
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="B14" s="54"/>
+        <v>164</v>
+      </c>
+      <c r="B14" s="53"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
@@ -4771,11 +4747,11 @@
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B15" s="54"/>
+        <v>161</v>
+      </c>
+      <c r="B15" s="53"/>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
@@ -4783,11 +4759,11 @@
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" s="54"/>
+        <v>165</v>
+      </c>
+      <c r="B16" s="53"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
@@ -4795,11 +4771,11 @@
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" s="54"/>
+        <v>166</v>
+      </c>
+      <c r="B17" s="53"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
@@ -4807,11 +4783,11 @@
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="B18" s="54"/>
+        <v>167</v>
+      </c>
+      <c r="B18" s="53"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
@@ -4819,11 +4795,11 @@
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
     </row>
-    <row r="19" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" s="54"/>
+        <v>168</v>
+      </c>
+      <c r="B19" s="53"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
@@ -4831,11 +4807,11 @@
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
     </row>
-    <row r="20" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="B20" s="54"/>
+        <v>169</v>
+      </c>
+      <c r="B20" s="53"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
@@ -4843,11 +4819,11 @@
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
     </row>
-    <row r="21" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B21" s="54"/>
+        <v>170</v>
+      </c>
+      <c r="B21" s="53"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
@@ -4855,9 +4831,9 @@
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
     </row>
-    <row r="22" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
-      <c r="B22" s="54"/>
+      <c r="B22" s="53"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
@@ -4865,9 +4841,9 @@
       <c r="G22" s="25"/>
       <c r="H22" s="25"/>
     </row>
-    <row r="23" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
-      <c r="B23" s="54"/>
+      <c r="B23" s="53"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
@@ -4875,9 +4851,9 @@
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
     </row>
-    <row r="24" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
-      <c r="B24" s="54"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
       <c r="E24" s="25"/>
@@ -4885,9 +4861,9 @@
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
     </row>
-    <row r="25" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
-      <c r="B25" s="54"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>
       <c r="E25" s="25"/>
@@ -4895,11 +4871,11 @@
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
     </row>
-    <row r="26" spans="1:8" s="53" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
-        <v>159</v>
-      </c>
-      <c r="B26" s="54"/>
+    <row r="26" spans="1:8" s="52" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="53"/>
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>
@@ -4907,11 +4883,11 @@
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
     </row>
-    <row r="27" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" s="54"/>
+        <v>161</v>
+      </c>
+      <c r="B27" s="53"/>
       <c r="C27" s="25"/>
       <c r="D27" s="25"/>
       <c r="E27" s="25"/>
@@ -4919,11 +4895,11 @@
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="B28" s="54"/>
+        <v>172</v>
+      </c>
+      <c r="B28" s="53"/>
       <c r="C28" s="25"/>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
@@ -4931,11 +4907,11 @@
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
     </row>
-    <row r="29" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="B29" s="54"/>
+        <v>173</v>
+      </c>
+      <c r="B29" s="53"/>
       <c r="C29" s="25"/>
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>
@@ -4943,11 +4919,11 @@
       <c r="G29" s="25"/>
       <c r="H29" s="25"/>
     </row>
-    <row r="30" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="B30" s="54"/>
+        <v>174</v>
+      </c>
+      <c r="B30" s="53"/>
       <c r="C30" s="25"/>
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
@@ -4955,11 +4931,11 @@
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
     </row>
-    <row r="31" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="B31" s="54"/>
+        <v>175</v>
+      </c>
+      <c r="B31" s="53"/>
       <c r="C31" s="25"/>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
@@ -4967,11 +4943,11 @@
       <c r="G31" s="25"/>
       <c r="H31" s="25"/>
     </row>
-    <row r="32" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="B32" s="54"/>
+        <v>176</v>
+      </c>
+      <c r="B32" s="53"/>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
@@ -4979,9 +4955,9 @@
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
     </row>
-    <row r="33" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
-      <c r="B33" s="54"/>
+      <c r="B33" s="53"/>
       <c r="C33" s="25"/>
       <c r="D33" s="25"/>
       <c r="E33" s="25"/>
@@ -4989,9 +4965,9 @@
       <c r="G33" s="25"/>
       <c r="H33" s="25"/>
     </row>
-    <row r="34" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
-      <c r="B34" s="54"/>
+      <c r="B34" s="53"/>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
       <c r="E34" s="25"/>
@@ -4999,9 +4975,9 @@
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
     </row>
-    <row r="35" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
-      <c r="B35" s="54"/>
+      <c r="B35" s="53"/>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
       <c r="E35" s="25"/>
@@ -5009,11 +4985,11 @@
       <c r="G35" s="25"/>
       <c r="H35" s="25"/>
     </row>
-    <row r="36" spans="1:8" s="53" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="96" t="s">
-        <v>165</v>
-      </c>
-      <c r="B36" s="54"/>
+    <row r="36" spans="1:8" s="52" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="87" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="53"/>
       <c r="C36" s="25"/>
       <c r="D36" s="25"/>
       <c r="E36" s="25"/>
@@ -5021,11 +4997,11 @@
       <c r="G36" s="25"/>
       <c r="H36" s="25"/>
     </row>
-    <row r="37" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="B37" s="54"/>
+        <v>178</v>
+      </c>
+      <c r="B37" s="53"/>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
@@ -5033,11 +5009,11 @@
       <c r="G37" s="25"/>
       <c r="H37" s="25"/>
     </row>
-    <row r="38" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="B38" s="54"/>
+        <v>179</v>
+      </c>
+      <c r="B38" s="53"/>
       <c r="C38" s="25"/>
       <c r="D38" s="25"/>
       <c r="E38" s="25"/>
@@ -5045,11 +5021,11 @@
       <c r="G38" s="25"/>
       <c r="H38" s="25"/>
     </row>
-    <row r="39" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="B39" s="54"/>
+        <v>180</v>
+      </c>
+      <c r="B39" s="53"/>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
       <c r="E39" s="25"/>
@@ -5057,11 +5033,11 @@
       <c r="G39" s="25"/>
       <c r="H39" s="25"/>
     </row>
-    <row r="40" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="B40" s="54"/>
+        <v>181</v>
+      </c>
+      <c r="B40" s="53"/>
       <c r="C40" s="25"/>
       <c r="D40" s="25"/>
       <c r="E40" s="25"/>
@@ -5069,11 +5045,11 @@
       <c r="G40" s="25"/>
       <c r="H40" s="25"/>
     </row>
-    <row r="41" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="B41" s="54"/>
+        <v>182</v>
+      </c>
+      <c r="B41" s="53"/>
       <c r="C41" s="25"/>
       <c r="D41" s="25"/>
       <c r="E41" s="25"/>
@@ -5081,11 +5057,11 @@
       <c r="G41" s="25"/>
       <c r="H41" s="25"/>
     </row>
-    <row r="42" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="B42" s="54"/>
+        <v>183</v>
+      </c>
+      <c r="B42" s="53"/>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
       <c r="E42" s="25"/>
@@ -5093,11 +5069,11 @@
       <c r="G42" s="25"/>
       <c r="H42" s="25"/>
     </row>
-    <row r="43" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="B43" s="54"/>
+        <v>184</v>
+      </c>
+      <c r="B43" s="53"/>
       <c r="C43" s="25"/>
       <c r="D43" s="25"/>
       <c r="E43" s="25"/>
@@ -5105,11 +5081,11 @@
       <c r="G43" s="25"/>
       <c r="H43" s="25"/>
     </row>
-    <row r="44" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="B44" s="54"/>
+        <v>185</v>
+      </c>
+      <c r="B44" s="53"/>
       <c r="C44" s="25"/>
       <c r="D44" s="25"/>
       <c r="E44" s="25"/>
@@ -5117,9 +5093,9 @@
       <c r="G44" s="25"/>
       <c r="H44" s="25"/>
     </row>
-    <row r="45" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
-      <c r="B45" s="54"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="25"/>
       <c r="D45" s="25"/>
       <c r="E45" s="25"/>
@@ -5128,94 +5104,94 @@
       <c r="H45" s="25"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="91" t="s">
-        <v>174</v>
-      </c>
-      <c r="B46" s="92">
+      <c r="A46" s="82" t="s">
+        <v>186</v>
+      </c>
+      <c r="B46" s="83">
         <f>SUBTOTAL(109,Table2[Total expenditure])</f>
         <v>0</v>
       </c>
-      <c r="C46" s="92">
+      <c r="C46" s="83">
         <f>SUBTOTAL(109,Table2[Non Core Expenditure])</f>
         <v>0</v>
       </c>
-      <c r="D46" s="92">
+      <c r="D46" s="83">
         <f>SUBTOTAL(109,Table2[Total Core Expenditure])</f>
         <v>0</v>
       </c>
-      <c r="E46" s="92">
+      <c r="E46" s="83">
         <f>SUBTOTAL(109,Table2[Total UK/EEA Core Expenditure])</f>
         <v>0</v>
       </c>
-      <c r="F46" s="92">
+      <c r="F46" s="83">
         <f>SUM(Table2[Total Non UK/EEA Core Expenditure])</f>
         <v>0</v>
       </c>
-      <c r="G46" s="92">
+      <c r="G46" s="83">
         <f>SUM(Table2[[Apportionment basis ]])</f>
         <v>0</v>
       </c>
-      <c r="H46" s="93"/>
-    </row>
-    <row r="47" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="51" t="s">
-        <v>175</v>
-      </c>
-      <c r="B47" s="56"/>
+      <c r="H46" s="84"/>
+    </row>
+    <row r="47" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="50" t="s">
+        <v>187</v>
+      </c>
+      <c r="B47" s="55"/>
       <c r="C47" s="26"/>
       <c r="D47" s="26"/>
-      <c r="E47" s="57"/>
+      <c r="E47" s="56"/>
       <c r="F47" s="26"/>
       <c r="G47" s="26"/>
-      <c r="H47" s="52"/>
+      <c r="H47" s="51"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="94" t="s">
-        <v>174</v>
-      </c>
-      <c r="B48" s="95">
+      <c r="A48" s="85" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48" s="86">
         <f>Table2[[#Totals],[Total expenditure]]-B47</f>
         <v>0</v>
       </c>
-      <c r="C48" s="95">
+      <c r="C48" s="86">
         <f>Table2[[#Totals],[Non Core Expenditure]]-C47</f>
         <v>0</v>
       </c>
-      <c r="D48" s="95">
+      <c r="D48" s="86">
         <f>Table2[[#Totals],[Total Core Expenditure]]-D47</f>
         <v>0</v>
       </c>
-      <c r="E48" s="95">
+      <c r="E48" s="86">
         <f>Table2[[#Totals],[Total UK/EEA Core Expenditure]]-E47</f>
         <v>0</v>
       </c>
-      <c r="F48" s="95">
+      <c r="F48" s="86">
         <f>Table2[[#Totals],[Total Non UK/EEA Core Expenditure]]-F47</f>
         <v>0</v>
       </c>
-      <c r="G48" s="95">
+      <c r="G48" s="86">
         <f>Table2[[#Totals],[Apportionment basis ]]-G47</f>
         <v>0</v>
       </c>
-      <c r="H48" s="95"/>
+      <c r="H48" s="86"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="58"/>
+      <c r="A106" s="57"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="8zHKp46lONSTxY+OVn2QmRb5KztwPgpzj5RdsBzFdf0UAKROBjnCch+/iBXXsBaEcf5lfnOAUI9QWHt3Gtn/zw==" saltValue="lvgv5htRvjFSbAI+YtFwBg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0"/>
@@ -5224,12 +5200,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="notEqual">
       <formula>$B$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="notEqual">
       <formula>$E$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5249,6 +5225,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43f61a81-08e4-450f-9189-2143ec144f36">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Notes xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
+    <Description xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
+    <Restricted_x003f_ xmlns="43f61a81-08e4-450f-9189-2143ec144f36">false</Restricted_x003f_>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Date xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
+    <_x0077_gy3 xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
+    <TaxCatchAll xmlns="229aab0b-7173-4521-96dd-bb43636f532e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5257,7 +5252,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FADE49AA34772468ECB203A2ABF3A84" ma:contentTypeVersion="31" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f4d253bc20ba4df7ac9ec746ac7562d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="43f61a81-08e4-450f-9189-2143ec144f36" xmlns:ns3="229aab0b-7173-4521-96dd-bb43636f532e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b47f16e74ed1ec9b37661be9f25fead" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5569,26 +5564,19 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="43f61a81-08e4-450f-9189-2143ec144f36">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Notes xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
-    <Description xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
-    <Restricted_x003f_ xmlns="43f61a81-08e4-450f-9189-2143ec144f36">false</Restricted_x003f_>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Date xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
-    <_x0077_gy3 xmlns="43f61a81-08e4-450f-9189-2143ec144f36" xsi:nil="true"/>
-    <TaxCatchAll xmlns="229aab0b-7173-4521-96dd-bb43636f532e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9762069-6060-41FB-BF07-1F90D25719D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="43f61a81-08e4-450f-9189-2143ec144f36"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="229aab0b-7173-4521-96dd-bb43636f532e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE4759-1A60-4A08-AC49-DF59832279FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -5596,7 +5584,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{350FA591-AFCC-4DF0-9191-454AADAFC530}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5614,22 +5602,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9762069-6060-41FB-BF07-1F90D25719D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="229aab0b-7173-4521-96dd-bb43636f532e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="43f61a81-08e4-450f-9189-2143ec144f36"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>